<commit_message>
additional tab for services
</commit_message>
<xml_diff>
--- a/documentation/DataAndAPIMatchAware.xlsx
+++ b/documentation/DataAndAPIMatchAware.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\match-aware\documentation\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16212" windowHeight="9060" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="UserEntities" sheetId="1" r:id="rId1"/>
@@ -26,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1570" uniqueCount="472">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1549" uniqueCount="484">
   <si>
     <t>USER</t>
   </si>
@@ -1442,12 +1447,48 @@
   </si>
   <si>
     <t>TEAM_MEMBERS</t>
+  </si>
+  <si>
+    <t>Services</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Desciprtion</t>
+  </si>
+  <si>
+    <t>AuthenticationService</t>
+  </si>
+  <si>
+    <t>UserService</t>
+  </si>
+  <si>
+    <t>authToken</t>
+  </si>
+  <si>
+    <t>JSON Web Token received upon authentication and used for all transactions with the API from that point forward.</t>
+  </si>
+  <si>
+    <t>loggedIn</t>
+  </si>
+  <si>
+    <t>Indication of whether the user has logged in to the system and been authenticated.  Used in the system to control display of elements selectively.</t>
+  </si>
+  <si>
+    <t>make club and user requred in REST API clubmember</t>
+  </si>
+  <si>
+    <t>ORGANIZATIONS not implemented</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1551,7 +1592,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="36">
     <border>
       <left/>
       <right/>
@@ -1979,11 +2020,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="115">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -2204,21 +2274,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -2248,39 +2303,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2293,6 +2315,57 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2599,7 +2672,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2609,69 +2682,69 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:W64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="A13" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.5703125" style="2" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="39.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="2.5703125" style="2" customWidth="1"/>
-    <col min="13" max="13" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="6.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="32.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="2.5703125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="9.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="16.85546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="17.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.5546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="39.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="2.5546875" style="2" customWidth="1"/>
+    <col min="13" max="13" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="32.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="5.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="2.5546875" style="2" customWidth="1"/>
+    <col min="19" max="19" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="9.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="16.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="21" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="101" t="s">
+    <row r="2" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="100" t="s">
         <v>441</v>
       </c>
-      <c r="B3" s="102"/>
-      <c r="C3" s="102"/>
-      <c r="D3" s="102"/>
-      <c r="E3" s="103"/>
+      <c r="B3" s="101"/>
+      <c r="C3" s="101"/>
+      <c r="D3" s="101"/>
+      <c r="E3" s="102"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="98" t="s">
+      <c r="G3" s="97" t="s">
         <v>433</v>
       </c>
-      <c r="H3" s="99"/>
-      <c r="I3" s="99"/>
-      <c r="J3" s="99"/>
-      <c r="K3" s="100"/>
-      <c r="M3" s="98" t="s">
+      <c r="H3" s="98"/>
+      <c r="I3" s="98"/>
+      <c r="J3" s="98"/>
+      <c r="K3" s="99"/>
+      <c r="M3" s="97" t="s">
         <v>430</v>
       </c>
-      <c r="N3" s="99"/>
-      <c r="O3" s="99"/>
-      <c r="P3" s="99"/>
-      <c r="Q3" s="100"/>
-    </row>
-    <row r="4" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N3" s="98"/>
+      <c r="O3" s="98"/>
+      <c r="P3" s="98"/>
+      <c r="Q3" s="99"/>
+    </row>
+    <row r="4" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="36" t="s">
         <v>1</v>
       </c>
@@ -2718,7 +2791,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="37" t="s">
         <v>16</v>
       </c>
@@ -2765,7 +2838,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6" s="38" t="s">
         <v>78</v>
       </c>
@@ -2802,7 +2875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7" s="38" t="s">
         <v>79</v>
       </c>
@@ -2837,7 +2910,7 @@
       <c r="P7" s="8"/>
       <c r="Q7" s="24"/>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
         <v>80</v>
       </c>
@@ -2870,7 +2943,7 @@
       <c r="P8" s="8"/>
       <c r="Q8" s="24"/>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9" s="38" t="s">
         <v>81</v>
       </c>
@@ -2901,7 +2974,7 @@
       <c r="P9" s="8"/>
       <c r="Q9" s="24"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10" s="38" t="s">
         <v>82</v>
       </c>
@@ -2936,7 +3009,7 @@
       <c r="P10" s="8"/>
       <c r="Q10" s="24"/>
     </row>
-    <row r="11" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="38" t="s">
         <v>83</v>
       </c>
@@ -2971,7 +3044,7 @@
       <c r="U11" s="51"/>
       <c r="W11" s="51"/>
     </row>
-    <row r="12" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="38" t="s">
         <v>43</v>
       </c>
@@ -3000,7 +3073,7 @@
       <c r="U12" s="51"/>
       <c r="W12" s="51"/>
     </row>
-    <row r="13" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="38" t="s">
         <v>44</v>
       </c>
@@ -3010,13 +3083,13 @@
       <c r="C13" s="21"/>
       <c r="D13" s="8"/>
       <c r="E13" s="24"/>
-      <c r="G13" s="98" t="s">
+      <c r="G13" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="H13" s="99"/>
-      <c r="I13" s="99"/>
-      <c r="J13" s="99"/>
-      <c r="K13" s="100"/>
+      <c r="H13" s="98"/>
+      <c r="I13" s="98"/>
+      <c r="J13" s="98"/>
+      <c r="K13" s="99"/>
       <c r="M13" s="10" t="s">
         <v>47</v>
       </c>
@@ -3029,7 +3102,7 @@
       <c r="U13" s="51"/>
       <c r="W13" s="51"/>
     </row>
-    <row r="14" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="38" t="s">
         <v>45</v>
       </c>
@@ -3066,7 +3139,7 @@
       <c r="U14" s="51"/>
       <c r="W14" s="51"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15" s="38" t="s">
         <v>84</v>
       </c>
@@ -3099,7 +3172,7 @@
       <c r="U15" s="51"/>
       <c r="W15" s="51"/>
     </row>
-    <row r="16" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
         <v>46</v>
       </c>
@@ -3132,7 +3205,7 @@
       <c r="U16" s="51"/>
       <c r="W16" s="51"/>
     </row>
-    <row r="17" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="10" t="s">
         <v>85</v>
       </c>
@@ -3156,7 +3229,7 @@
       <c r="U17" s="51"/>
       <c r="W17" s="51"/>
     </row>
-    <row r="18" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="10" t="s">
         <v>159</v>
       </c>
@@ -3168,13 +3241,13 @@
         <v>160</v>
       </c>
       <c r="E18" s="24"/>
-      <c r="G18" s="98" t="s">
+      <c r="G18" s="97" t="s">
         <v>434</v>
       </c>
-      <c r="H18" s="99"/>
-      <c r="I18" s="99"/>
-      <c r="J18" s="99"/>
-      <c r="K18" s="100"/>
+      <c r="H18" s="98"/>
+      <c r="I18" s="98"/>
+      <c r="J18" s="98"/>
+      <c r="K18" s="99"/>
       <c r="M18" s="10" t="s">
         <v>53</v>
       </c>
@@ -3187,7 +3260,7 @@
       <c r="U18" s="51"/>
       <c r="W18" s="51"/>
     </row>
-    <row r="19" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="10" t="s">
         <v>161</v>
       </c>
@@ -3226,7 +3299,7 @@
       <c r="U19" s="51"/>
       <c r="W19" s="51"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>86</v>
       </c>
@@ -3263,7 +3336,7 @@
       <c r="U20" s="51"/>
       <c r="W20" s="51"/>
     </row>
-    <row r="21" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21" s="13" t="s">
         <v>87</v>
       </c>
@@ -3296,7 +3369,7 @@
       <c r="U21" s="51"/>
       <c r="W21" s="51"/>
     </row>
-    <row r="22" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G22" s="16"/>
       <c r="H22" s="41"/>
       <c r="I22" s="30"/>
@@ -3314,21 +3387,21 @@
       <c r="U22" s="51"/>
       <c r="W22" s="51"/>
     </row>
-    <row r="23" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="104" t="s">
+    <row r="23" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="103" t="s">
         <v>442</v>
       </c>
-      <c r="B23" s="105"/>
-      <c r="C23" s="105"/>
-      <c r="D23" s="105"/>
-      <c r="E23" s="106"/>
-      <c r="G23" s="101" t="s">
+      <c r="B23" s="104"/>
+      <c r="C23" s="104"/>
+      <c r="D23" s="104"/>
+      <c r="E23" s="105"/>
+      <c r="G23" s="100" t="s">
         <v>443</v>
       </c>
-      <c r="H23" s="102"/>
-      <c r="I23" s="102"/>
-      <c r="J23" s="102"/>
-      <c r="K23" s="103"/>
+      <c r="H23" s="101"/>
+      <c r="I23" s="101"/>
+      <c r="J23" s="101"/>
+      <c r="K23" s="102"/>
       <c r="M23" s="10" t="s">
         <v>58</v>
       </c>
@@ -3341,7 +3414,7 @@
       <c r="U23" s="51"/>
       <c r="W23" s="51"/>
     </row>
-    <row r="24" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A24" s="17" t="s">
         <v>1</v>
       </c>
@@ -3384,7 +3457,7 @@
       <c r="U24" s="51"/>
       <c r="W24" s="51"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>91</v>
       </c>
@@ -3425,7 +3498,7 @@
       <c r="U25" s="51"/>
       <c r="W25" s="51"/>
     </row>
-    <row r="26" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="13" t="s">
         <v>92</v>
       </c>
@@ -3462,7 +3535,7 @@
       <c r="U26" s="51"/>
       <c r="W26" s="51"/>
     </row>
-    <row r="27" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A27" s="16"/>
       <c r="B27" s="16"/>
       <c r="C27" s="16"/>
@@ -3492,14 +3565,14 @@
       <c r="Q27" s="9"/>
       <c r="W27" s="51"/>
     </row>
-    <row r="28" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="104" t="s">
+    <row r="28" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="103" t="s">
         <v>439</v>
       </c>
-      <c r="B28" s="105"/>
-      <c r="C28" s="105"/>
-      <c r="D28" s="105"/>
-      <c r="E28" s="106"/>
+      <c r="B28" s="104"/>
+      <c r="C28" s="104"/>
+      <c r="D28" s="104"/>
+      <c r="E28" s="105"/>
       <c r="G28" s="13" t="s">
         <v>12</v>
       </c>
@@ -3522,7 +3595,7 @@
       <c r="Q28" s="9"/>
       <c r="W28" s="51"/>
     </row>
-    <row r="29" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="17" t="s">
         <v>1</v>
       </c>
@@ -3540,7 +3613,7 @@
       </c>
       <c r="W29" s="51"/>
     </row>
-    <row r="30" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>16</v>
       </c>
@@ -3556,22 +3629,22 @@
       <c r="E30" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G30" s="98" t="s">
+      <c r="G30" s="97" t="s">
         <v>15</v>
       </c>
-      <c r="H30" s="99"/>
-      <c r="I30" s="99"/>
-      <c r="J30" s="99"/>
-      <c r="K30" s="100"/>
-      <c r="M30" s="98" t="s">
+      <c r="H30" s="98"/>
+      <c r="I30" s="98"/>
+      <c r="J30" s="98"/>
+      <c r="K30" s="99"/>
+      <c r="M30" s="97" t="s">
         <v>431</v>
       </c>
-      <c r="N30" s="99"/>
-      <c r="O30" s="99"/>
-      <c r="P30" s="99"/>
-      <c r="Q30" s="100"/>
-    </row>
-    <row r="31" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N30" s="98"/>
+      <c r="O30" s="98"/>
+      <c r="P30" s="98"/>
+      <c r="Q30" s="99"/>
+    </row>
+    <row r="31" spans="1:23" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A31" s="10" t="s">
         <v>12</v>
       </c>
@@ -3618,7 +3691,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="8"/>
       <c r="C32" s="8"/>
@@ -3651,7 +3724,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33" s="10"/>
       <c r="B33" s="8"/>
       <c r="C33" s="8"/>
@@ -3682,7 +3755,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34" s="10"/>
       <c r="B34" s="8"/>
       <c r="C34" s="8"/>
@@ -3711,7 +3784,7 @@
       <c r="P34" s="8"/>
       <c r="Q34" s="29"/>
     </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35" s="10"/>
       <c r="B35" s="8"/>
       <c r="C35" s="8"/>
@@ -3740,7 +3813,7 @@
       <c r="P35" s="8"/>
       <c r="Q35" s="29"/>
     </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36" s="10"/>
       <c r="B36" s="8"/>
       <c r="C36" s="8"/>
@@ -3767,7 +3840,7 @@
       <c r="P36" s="8"/>
       <c r="Q36" s="9"/>
     </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37" s="10"/>
       <c r="B37" s="8"/>
       <c r="C37" s="8"/>
@@ -3794,7 +3867,7 @@
       <c r="P37" s="8"/>
       <c r="Q37" s="9"/>
     </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38" s="10"/>
       <c r="B38" s="8"/>
       <c r="C38" s="8"/>
@@ -3821,7 +3894,7 @@
       <c r="P38" s="8"/>
       <c r="Q38" s="9"/>
     </row>
-    <row r="39" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="13"/>
       <c r="B39" s="14"/>
       <c r="C39" s="14"/>
@@ -3848,7 +3921,7 @@
       <c r="P39" s="8"/>
       <c r="Q39" s="9"/>
     </row>
-    <row r="40" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="F40" s="16"/>
       <c r="G40" s="10" t="s">
         <v>32</v>
@@ -3869,14 +3942,14 @@
       <c r="P40" s="8"/>
       <c r="Q40" s="9"/>
     </row>
-    <row r="41" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="98" t="s">
+    <row r="41" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="97" t="s">
         <v>440</v>
       </c>
-      <c r="B41" s="99"/>
-      <c r="C41" s="99"/>
-      <c r="D41" s="99"/>
-      <c r="E41" s="100"/>
+      <c r="B41" s="98"/>
+      <c r="C41" s="98"/>
+      <c r="D41" s="98"/>
+      <c r="E41" s="99"/>
       <c r="G41" s="10" t="s">
         <v>33</v>
       </c>
@@ -3898,7 +3971,7 @@
       </c>
       <c r="Q41" s="15"/>
     </row>
-    <row r="42" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A42" s="17" t="s">
         <v>1</v>
       </c>
@@ -3924,7 +3997,7 @@
       <c r="J42" s="8"/>
       <c r="K42" s="9"/>
     </row>
-    <row r="43" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="4" t="s">
         <v>16</v>
       </c>
@@ -3949,26 +4022,26 @@
       <c r="I43" s="8"/>
       <c r="J43" s="8"/>
       <c r="K43" s="9"/>
-      <c r="M43" s="98" t="s">
+      <c r="M43" s="97" t="s">
         <v>432</v>
       </c>
-      <c r="N43" s="99"/>
-      <c r="O43" s="99"/>
-      <c r="P43" s="99"/>
-      <c r="Q43" s="100"/>
-    </row>
-    <row r="44" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="N43" s="98"/>
+      <c r="O43" s="98"/>
+      <c r="P43" s="98"/>
+      <c r="Q43" s="99"/>
+    </row>
+    <row r="44" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A44" s="43" t="s">
         <v>12</v>
       </c>
       <c r="B44" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C44" s="96" t="s">
+      <c r="C44" s="89" t="s">
         <v>5</v>
       </c>
       <c r="D44" s="46"/>
-      <c r="E44" s="97"/>
+      <c r="E44" s="90"/>
       <c r="G44" s="10" t="s">
         <v>36</v>
       </c>
@@ -3994,7 +4067,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45" s="10" t="s">
         <v>449</v>
       </c>
@@ -4031,7 +4104,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A46" s="10" t="s">
         <v>18</v>
       </c>
@@ -4066,7 +4139,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="47" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="M47" s="10" t="s">
         <v>65</v>
       </c>
@@ -4077,21 +4150,21 @@
       <c r="P47" s="8"/>
       <c r="Q47" s="29"/>
     </row>
-    <row r="48" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="98" t="s">
+    <row r="48" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="97" t="s">
         <v>444</v>
       </c>
-      <c r="B48" s="99"/>
-      <c r="C48" s="99"/>
-      <c r="D48" s="99"/>
-      <c r="E48" s="100"/>
-      <c r="G48" s="101" t="s">
+      <c r="B48" s="98"/>
+      <c r="C48" s="98"/>
+      <c r="D48" s="98"/>
+      <c r="E48" s="99"/>
+      <c r="G48" s="100" t="s">
         <v>437</v>
       </c>
-      <c r="H48" s="102"/>
-      <c r="I48" s="102"/>
-      <c r="J48" s="102"/>
-      <c r="K48" s="103"/>
+      <c r="H48" s="101"/>
+      <c r="I48" s="101"/>
+      <c r="J48" s="101"/>
+      <c r="K48" s="102"/>
       <c r="M48" s="10" t="s">
         <v>66</v>
       </c>
@@ -4102,7 +4175,7 @@
       <c r="P48" s="8"/>
       <c r="Q48" s="9"/>
     </row>
-    <row r="49" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A49" s="17" t="s">
         <v>1</v>
       </c>
@@ -4143,7 +4216,7 @@
       <c r="P49" s="8"/>
       <c r="Q49" s="9"/>
     </row>
-    <row r="50" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
         <v>16</v>
       </c>
@@ -4184,7 +4257,7 @@
       <c r="P50" s="14"/>
       <c r="Q50" s="15"/>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>12</v>
       </c>
@@ -4208,7 +4281,7 @@
       <c r="J51" s="8"/>
       <c r="K51" s="24"/>
     </row>
-    <row r="52" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A52" s="13" t="s">
         <v>169</v>
       </c>
@@ -4232,7 +4305,7 @@
       </c>
       <c r="K52" s="24"/>
     </row>
-    <row r="53" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G53" s="10"/>
       <c r="H53" s="8"/>
       <c r="I53" s="8"/>
@@ -4241,14 +4314,14 @@
       </c>
       <c r="K53" s="24"/>
     </row>
-    <row r="54" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="98" t="s">
+    <row r="54" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="97" t="s">
         <v>445</v>
       </c>
-      <c r="B54" s="99"/>
-      <c r="C54" s="99"/>
-      <c r="D54" s="99"/>
-      <c r="E54" s="100"/>
+      <c r="B54" s="98"/>
+      <c r="C54" s="98"/>
+      <c r="D54" s="98"/>
+      <c r="E54" s="99"/>
       <c r="G54" s="10"/>
       <c r="H54" s="8"/>
       <c r="I54" s="8"/>
@@ -4257,7 +4330,7 @@
       </c>
       <c r="K54" s="24"/>
     </row>
-    <row r="55" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="17" t="s">
         <v>1</v>
       </c>
@@ -4280,12 +4353,12 @@
         <v>438</v>
       </c>
       <c r="I55" s="14"/>
-      <c r="J55" s="87">
+      <c r="J55" s="80">
         <v>0</v>
       </c>
       <c r="K55" s="25"/>
     </row>
-    <row r="56" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="4" t="s">
         <v>104</v>
       </c>
@@ -4298,7 +4371,7 @@
       <c r="D56" s="6"/>
       <c r="E56" s="28"/>
     </row>
-    <row r="57" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A57" s="10" t="s">
         <v>0</v>
       </c>
@@ -4310,15 +4383,15 @@
       </c>
       <c r="D57" s="8"/>
       <c r="E57" s="29"/>
-      <c r="G57" s="98" t="s">
+      <c r="G57" s="97" t="s">
         <v>436</v>
       </c>
-      <c r="H57" s="99"/>
-      <c r="I57" s="99"/>
-      <c r="J57" s="99"/>
-      <c r="K57" s="100"/>
-    </row>
-    <row r="58" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H57" s="98"/>
+      <c r="I57" s="98"/>
+      <c r="J57" s="98"/>
+      <c r="K57" s="99"/>
+    </row>
+    <row r="58" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G58" s="17" t="s">
         <v>1</v>
       </c>
@@ -4335,14 +4408,14 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="98" t="s">
+    <row r="59" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="97" t="s">
         <v>471</v>
       </c>
-      <c r="B59" s="99"/>
-      <c r="C59" s="99"/>
-      <c r="D59" s="99"/>
-      <c r="E59" s="100"/>
+      <c r="B59" s="98"/>
+      <c r="C59" s="98"/>
+      <c r="D59" s="98"/>
+      <c r="E59" s="99"/>
       <c r="G59" s="4" t="s">
         <v>16</v>
       </c>
@@ -4359,7 +4432,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="60" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A60" s="17" t="s">
         <v>1</v>
       </c>
@@ -4387,7 +4460,7 @@
       <c r="J60" s="8"/>
       <c r="K60" s="24"/>
     </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A61" s="4" t="s">
         <v>103</v>
       </c>
@@ -4409,7 +4482,7 @@
       <c r="J61" s="8"/>
       <c r="K61" s="24"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>106</v>
       </c>
@@ -4431,7 +4504,7 @@
       <c r="J62" s="8"/>
       <c r="K62" s="24"/>
     </row>
-    <row r="63" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>93</v>
       </c>
@@ -4453,7 +4526,7 @@
       <c r="J63" s="8"/>
       <c r="K63" s="24"/>
     </row>
-    <row r="64" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:17" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="G64" s="13" t="s">
         <v>171</v>
       </c>
@@ -4466,13 +4539,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="M30:Q30"/>
-    <mergeCell ref="M3:Q3"/>
-    <mergeCell ref="M43:Q43"/>
-    <mergeCell ref="A3:E3"/>
-    <mergeCell ref="G3:K3"/>
-    <mergeCell ref="G18:K18"/>
-    <mergeCell ref="G13:K13"/>
+    <mergeCell ref="G57:K57"/>
+    <mergeCell ref="A59:E59"/>
     <mergeCell ref="A48:E48"/>
     <mergeCell ref="A54:E54"/>
     <mergeCell ref="G48:K48"/>
@@ -4481,8 +4549,13 @@
     <mergeCell ref="A23:E23"/>
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A41:E41"/>
-    <mergeCell ref="G57:K57"/>
-    <mergeCell ref="A59:E59"/>
+    <mergeCell ref="M30:Q30"/>
+    <mergeCell ref="M3:Q3"/>
+    <mergeCell ref="M43:Q43"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="G3:K3"/>
+    <mergeCell ref="G18:K18"/>
+    <mergeCell ref="G13:K13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -4497,27 +4570,27 @@
       <selection activeCell="A66" sqref="A66:E70"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="27.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" style="51" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" style="51" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="49.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.88671875" style="51" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" style="51" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="49.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="101" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="100" t="s">
         <v>110</v>
       </c>
-      <c r="B1" s="102"/>
-      <c r="C1" s="102"/>
-      <c r="D1" s="102"/>
-      <c r="E1" s="103"/>
-    </row>
-    <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="101"/>
+      <c r="C1" s="101"/>
+      <c r="D1" s="101"/>
+      <c r="E1" s="102"/>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>1</v>
       </c>
@@ -4534,7 +4607,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>16</v>
       </c>
@@ -4551,7 +4624,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
@@ -4564,7 +4637,7 @@
       <c r="D4" s="8"/>
       <c r="E4" s="24"/>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>104</v>
       </c>
@@ -4577,7 +4650,7 @@
       <c r="D5" s="8"/>
       <c r="E5" s="24"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>93</v>
       </c>
@@ -4590,7 +4663,7 @@
       <c r="D6" s="8"/>
       <c r="E6" s="24"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="10" t="s">
         <v>103</v>
       </c>
@@ -4601,7 +4674,7 @@
       <c r="D7" s="8"/>
       <c r="E7" s="24"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>111</v>
       </c>
@@ -4614,7 +4687,7 @@
       </c>
       <c r="E8" s="24"/>
     </row>
-    <row r="9" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="13" t="s">
         <v>113</v>
       </c>
@@ -4627,17 +4700,17 @@
       </c>
       <c r="E9" s="25"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="101" t="s">
+    <row r="10" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="11" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="100" t="s">
         <v>115</v>
       </c>
-      <c r="B11" s="102"/>
-      <c r="C11" s="102"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="103"/>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="101"/>
+      <c r="C11" s="101"/>
+      <c r="D11" s="101"/>
+      <c r="E11" s="102"/>
+    </row>
+    <row r="12" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>1</v>
       </c>
@@ -4654,7 +4727,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>16</v>
       </c>
@@ -4671,7 +4744,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>12</v>
       </c>
@@ -4687,17 +4760,17 @@
       </c>
       <c r="G14" s="53"/>
     </row>
-    <row r="15" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="16" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="101" t="s">
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="16" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="100" t="s">
         <v>116</v>
       </c>
-      <c r="B16" s="102"/>
-      <c r="C16" s="102"/>
-      <c r="D16" s="102"/>
-      <c r="E16" s="103"/>
-    </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="101"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="101"/>
+      <c r="E16" s="102"/>
+    </row>
+    <row r="17" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="17" t="s">
         <v>1</v>
       </c>
@@ -4714,7 +4787,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
         <v>16</v>
       </c>
@@ -4731,7 +4804,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
         <v>12</v>
       </c>
@@ -4742,7 +4815,7 @@
       <c r="D19" s="8"/>
       <c r="E19" s="24"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
         <v>14</v>
       </c>
@@ -4755,7 +4828,7 @@
       <c r="D20" s="8"/>
       <c r="E20" s="24"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="10" t="s">
         <v>118</v>
       </c>
@@ -4766,7 +4839,7 @@
       <c r="D21" s="8"/>
       <c r="E21" s="24"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
         <v>117</v>
       </c>
@@ -4777,7 +4850,7 @@
       <c r="D22" s="8"/>
       <c r="E22" s="24"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="10" t="s">
         <v>10</v>
       </c>
@@ -4788,7 +4861,7 @@
       <c r="D23" s="8"/>
       <c r="E23" s="24"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
         <v>122</v>
       </c>
@@ -4802,7 +4875,7 @@
       <c r="E24" s="24"/>
       <c r="I24" s="52"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
         <v>13</v>
       </c>
@@ -4813,7 +4886,7 @@
       <c r="D25" s="8"/>
       <c r="E25" s="24"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
         <v>11</v>
       </c>
@@ -4824,7 +4897,7 @@
       <c r="D26" s="8"/>
       <c r="E26" s="24"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
         <v>135</v>
       </c>
@@ -4835,7 +4908,7 @@
       <c r="D27" s="8"/>
       <c r="E27" s="24"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="10" t="s">
         <v>136</v>
       </c>
@@ -4846,7 +4919,7 @@
       <c r="D28" s="8"/>
       <c r="E28" s="24"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="10" t="s">
         <v>121</v>
       </c>
@@ -4857,7 +4930,7 @@
       <c r="D29" s="8"/>
       <c r="E29" s="24"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="10" t="s">
         <v>137</v>
       </c>
@@ -4868,7 +4941,7 @@
       <c r="D30" s="8"/>
       <c r="E30" s="24"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="10" t="s">
         <v>69</v>
       </c>
@@ -4879,7 +4952,7 @@
       <c r="D31" s="8"/>
       <c r="E31" s="24"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="10" t="s">
         <v>150</v>
       </c>
@@ -4890,7 +4963,7 @@
       <c r="D32" s="8"/>
       <c r="E32" s="24"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" s="10" t="s">
         <v>119</v>
       </c>
@@ -4901,7 +4974,7 @@
       <c r="D33" s="8"/>
       <c r="E33" s="24"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" s="10" t="s">
         <v>113</v>
       </c>
@@ -4914,7 +4987,7 @@
       </c>
       <c r="E34" s="24"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" s="60" t="s">
         <v>148</v>
       </c>
@@ -4925,7 +4998,7 @@
       <c r="D35" s="54"/>
       <c r="E35" s="61"/>
     </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A36" s="13" t="s">
         <v>138</v>
       </c>
@@ -4938,23 +5011,23 @@
       </c>
       <c r="E36" s="25"/>
     </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="16"/>
       <c r="B37" s="16"/>
       <c r="C37" s="30"/>
       <c r="D37" s="16"/>
       <c r="E37" s="30"/>
     </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="101" t="s">
+    <row r="38" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="100" t="s">
         <v>429</v>
       </c>
-      <c r="B38" s="102"/>
-      <c r="C38" s="102"/>
-      <c r="D38" s="102"/>
-      <c r="E38" s="103"/>
-    </row>
-    <row r="39" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B38" s="101"/>
+      <c r="C38" s="101"/>
+      <c r="D38" s="101"/>
+      <c r="E38" s="102"/>
+    </row>
+    <row r="39" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A39" s="17" t="s">
         <v>1</v>
       </c>
@@ -4971,7 +5044,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" s="4" t="s">
         <v>16</v>
       </c>
@@ -4988,7 +5061,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" s="10" t="s">
         <v>145</v>
       </c>
@@ -5001,7 +5074,7 @@
       <c r="D41" s="8"/>
       <c r="E41" s="24"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" s="10" t="s">
         <v>146</v>
       </c>
@@ -5014,7 +5087,7 @@
       <c r="D42" s="8"/>
       <c r="E42" s="24"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" s="60" t="s">
         <v>113</v>
       </c>
@@ -5027,7 +5100,7 @@
       </c>
       <c r="E43" s="61"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" s="60" t="s">
         <v>157</v>
       </c>
@@ -5040,7 +5113,7 @@
       <c r="D44" s="54"/>
       <c r="E44" s="61"/>
     </row>
-    <row r="45" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A45" s="13" t="s">
         <v>147</v>
       </c>
@@ -5056,17 +5129,17 @@
         <v>158</v>
       </c>
     </row>
-    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="101" t="s">
+    <row r="46" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="47" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="100" t="s">
         <v>435</v>
       </c>
-      <c r="B47" s="102"/>
-      <c r="C47" s="102"/>
-      <c r="D47" s="102"/>
-      <c r="E47" s="103"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B47" s="101"/>
+      <c r="C47" s="101"/>
+      <c r="D47" s="101"/>
+      <c r="E47" s="102"/>
+    </row>
+    <row r="48" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A48" s="17" t="s">
         <v>1</v>
       </c>
@@ -5083,7 +5156,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="4" t="s">
         <v>16</v>
       </c>
@@ -5100,7 +5173,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="10" t="s">
         <v>113</v>
       </c>
@@ -5115,7 +5188,7 @@
       </c>
       <c r="E50" s="24"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
         <v>14</v>
       </c>
@@ -5130,7 +5203,7 @@
       </c>
       <c r="E51" s="24"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="10" t="s">
         <v>116</v>
       </c>
@@ -5141,7 +5214,7 @@
       <c r="D52" s="8"/>
       <c r="E52" s="24"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="10" t="s">
         <v>155</v>
       </c>
@@ -5152,7 +5225,7 @@
       <c r="D53" s="8"/>
       <c r="E53" s="24"/>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="10" t="s">
         <v>152</v>
       </c>
@@ -5163,7 +5236,7 @@
       <c r="D54" s="8"/>
       <c r="E54" s="24"/>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="10" t="s">
         <v>153</v>
       </c>
@@ -5174,7 +5247,7 @@
       <c r="D55" s="8"/>
       <c r="E55" s="24"/>
     </row>
-    <row r="56" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
         <v>154</v>
       </c>
@@ -5185,17 +5258,17 @@
       <c r="D56" s="14"/>
       <c r="E56" s="25"/>
     </row>
-    <row r="57" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="101" t="s">
+    <row r="57" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="58" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="100" t="s">
         <v>173</v>
       </c>
-      <c r="B58" s="102"/>
-      <c r="C58" s="102"/>
-      <c r="D58" s="102"/>
-      <c r="E58" s="103"/>
-    </row>
-    <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="101"/>
+      <c r="C58" s="101"/>
+      <c r="D58" s="101"/>
+      <c r="E58" s="102"/>
+    </row>
+    <row r="59" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A59" s="17" t="s">
         <v>1</v>
       </c>
@@ -5212,7 +5285,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="4" t="s">
         <v>16</v>
       </c>
@@ -5229,7 +5302,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="10" t="s">
         <v>116</v>
       </c>
@@ -5240,7 +5313,7 @@
       <c r="D61" s="8"/>
       <c r="E61" s="24"/>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="10" t="s">
         <v>155</v>
       </c>
@@ -5251,7 +5324,7 @@
       <c r="D62" s="8"/>
       <c r="E62" s="24"/>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="10" t="s">
         <v>153</v>
       </c>
@@ -5262,7 +5335,7 @@
       <c r="D63" s="8"/>
       <c r="E63" s="24"/>
     </row>
-    <row r="64" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>154</v>
       </c>
@@ -5273,17 +5346,17 @@
       <c r="D64" s="14"/>
       <c r="E64" s="25"/>
     </row>
-    <row r="65" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="66" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="104" t="s">
+    <row r="65" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="66" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="103" t="s">
         <v>163</v>
       </c>
-      <c r="B66" s="105"/>
-      <c r="C66" s="105"/>
-      <c r="D66" s="105"/>
-      <c r="E66" s="106"/>
-    </row>
-    <row r="67" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B66" s="104"/>
+      <c r="C66" s="104"/>
+      <c r="D66" s="104"/>
+      <c r="E66" s="105"/>
+    </row>
+    <row r="67" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="48" t="s">
         <v>1</v>
       </c>
@@ -5300,7 +5373,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A68" s="43" t="s">
         <v>16</v>
       </c>
@@ -5317,7 +5390,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A69" s="10" t="s">
         <v>0</v>
       </c>
@@ -5328,7 +5401,7 @@
       <c r="D69" s="8"/>
       <c r="E69" s="24"/>
     </row>
-    <row r="70" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A70" s="13" t="s">
         <v>164</v>
       </c>
@@ -5341,17 +5414,17 @@
       </c>
       <c r="E70" s="25"/>
     </row>
-    <row r="71" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="72" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="104" t="s">
+    <row r="71" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="72" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A72" s="103" t="s">
         <v>174</v>
       </c>
-      <c r="B72" s="105"/>
-      <c r="C72" s="105"/>
-      <c r="D72" s="105"/>
-      <c r="E72" s="106"/>
-    </row>
-    <row r="73" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B72" s="104"/>
+      <c r="C72" s="104"/>
+      <c r="D72" s="104"/>
+      <c r="E72" s="105"/>
+    </row>
+    <row r="73" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A73" s="17" t="s">
         <v>1</v>
       </c>
@@ -5368,7 +5441,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A74" s="4" t="s">
         <v>16</v>
       </c>
@@ -5385,7 +5458,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A75" s="10" t="s">
         <v>165</v>
       </c>
@@ -5400,7 +5473,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A76" s="10" t="s">
         <v>167</v>
       </c>
@@ -5411,7 +5484,7 @@
       <c r="D76" s="8"/>
       <c r="E76" s="24"/>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A77" s="10" t="s">
         <v>168</v>
       </c>
@@ -5422,7 +5495,7 @@
       <c r="D77" s="8"/>
       <c r="E77" s="24"/>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A78" s="10" t="s">
         <v>93</v>
       </c>
@@ -5435,7 +5508,7 @@
       <c r="D78" s="8"/>
       <c r="E78" s="24"/>
     </row>
-    <row r="79" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A79" s="13" t="s">
         <v>113</v>
       </c>
@@ -5476,21 +5549,21 @@
       <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="46.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="39.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="46.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="107" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="106" t="s">
         <v>141</v>
       </c>
-      <c r="B1" s="108"/>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B1" s="107"/>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="56" t="s">
         <v>139</v>
       </c>
@@ -5498,7 +5571,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="56" t="s">
         <v>125</v>
       </c>
@@ -5506,7 +5579,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="56" t="s">
         <v>128</v>
       </c>
@@ -5514,7 +5587,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="56" t="s">
         <v>127</v>
       </c>
@@ -5522,7 +5595,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="56" t="s">
         <v>129</v>
       </c>
@@ -5530,7 +5603,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="56" t="s">
         <v>131</v>
       </c>
@@ -5538,7 +5611,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="58" t="s">
         <v>133</v>
       </c>
@@ -5561,32 +5634,33 @@
   </sheetPr>
   <dimension ref="A1:G173"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="A143" sqref="A143:F143"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.28515625" style="66" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="43.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="63.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.28515625" style="66" customWidth="1"/>
-    <col min="6" max="6" width="8.42578125" style="66" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" style="66" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="63.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.33203125" style="66" customWidth="1"/>
+    <col min="6" max="6" width="8.44140625" style="66" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="80" t="s">
+    <row r="1" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="108" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="81"/>
-      <c r="C1" s="81"/>
-      <c r="D1" s="81"/>
-      <c r="E1" s="81"/>
-      <c r="F1" s="82"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B1" s="109"/>
+      <c r="C1" s="109"/>
+      <c r="D1" s="109"/>
+      <c r="E1" s="109"/>
+      <c r="F1" s="109"/>
+      <c r="G1" s="109"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="67" t="s">
         <v>176</v>
       </c>
@@ -5605,11 +5679,11 @@
       <c r="F2" s="69" t="s">
         <v>405</v>
       </c>
-      <c r="G2" s="88" t="s">
+      <c r="G2" s="81" t="s">
         <v>446</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="70" t="s">
         <v>110</v>
       </c>
@@ -5629,7 +5703,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="70" t="s">
         <v>110</v>
       </c>
@@ -5649,7 +5723,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="70" t="s">
         <v>110</v>
       </c>
@@ -5667,7 +5741,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="70" t="s">
         <v>110</v>
       </c>
@@ -5685,7 +5759,7 @@
       </c>
       <c r="F6" s="77"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="70" t="s">
         <v>110</v>
       </c>
@@ -5703,7 +5777,7 @@
       </c>
       <c r="F7" s="77"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="70" t="s">
         <v>110</v>
       </c>
@@ -5719,7 +5793,7 @@
       <c r="E8" s="70"/>
       <c r="F8" s="77"/>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="71" t="s">
         <v>110</v>
       </c>
@@ -5737,7 +5811,7 @@
       </c>
       <c r="F9" s="76"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="71" t="s">
         <v>110</v>
       </c>
@@ -5755,7 +5829,7 @@
       </c>
       <c r="F10" s="76"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="70" t="s">
         <v>18</v>
       </c>
@@ -5773,7 +5847,7 @@
       </c>
       <c r="F11" s="77"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="70" t="s">
         <v>18</v>
       </c>
@@ -5793,7 +5867,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="70" t="s">
         <v>18</v>
       </c>
@@ -5809,7 +5883,7 @@
       <c r="E13" s="70"/>
       <c r="F13" s="77"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="70" t="s">
         <v>18</v>
       </c>
@@ -5827,7 +5901,7 @@
       </c>
       <c r="F14" s="77"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="70" t="s">
         <v>18</v>
       </c>
@@ -5847,7 +5921,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="70" t="s">
         <v>18</v>
       </c>
@@ -5863,7 +5937,7 @@
       <c r="E16" s="70"/>
       <c r="F16" s="77"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="70" t="s">
         <v>142</v>
       </c>
@@ -5883,7 +5957,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="70" t="s">
         <v>142</v>
       </c>
@@ -5903,7 +5977,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="70" t="s">
         <v>142</v>
       </c>
@@ -5921,7 +5995,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="70" t="s">
         <v>142</v>
       </c>
@@ -5939,7 +6013,7 @@
       </c>
       <c r="F20" s="77"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="70" t="s">
         <v>142</v>
       </c>
@@ -5959,7 +6033,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="70" t="s">
         <v>142</v>
       </c>
@@ -5975,7 +6049,7 @@
       <c r="E22" s="70"/>
       <c r="F22" s="77"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" s="70" t="s">
         <v>142</v>
       </c>
@@ -5993,7 +6067,7 @@
       </c>
       <c r="F23" s="77"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" s="70" t="s">
         <v>142</v>
       </c>
@@ -6011,7 +6085,7 @@
       </c>
       <c r="F24" s="77"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="70" t="s">
         <v>104</v>
       </c>
@@ -6029,7 +6103,7 @@
       </c>
       <c r="F25" s="77"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" s="70" t="s">
         <v>104</v>
       </c>
@@ -6049,7 +6123,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="70" t="s">
         <v>104</v>
       </c>
@@ -6065,7 +6139,7 @@
       <c r="E27" s="70"/>
       <c r="F27" s="77"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" s="70" t="s">
         <v>104</v>
       </c>
@@ -6083,7 +6157,7 @@
       </c>
       <c r="F28" s="77"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" s="70" t="s">
         <v>104</v>
       </c>
@@ -6103,7 +6177,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="70" t="s">
         <v>104</v>
       </c>
@@ -6119,7 +6193,7 @@
       <c r="E30" s="70"/>
       <c r="F30" s="77"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" s="70" t="s">
         <v>105</v>
       </c>
@@ -6139,7 +6213,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="70" t="s">
         <v>105</v>
       </c>
@@ -6157,7 +6231,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" s="70" t="s">
         <v>105</v>
       </c>
@@ -6175,7 +6249,7 @@
       </c>
       <c r="F33" s="77"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="70" t="s">
         <v>105</v>
       </c>
@@ -6193,7 +6267,7 @@
       </c>
       <c r="F34" s="77"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="70" t="s">
         <v>116</v>
       </c>
@@ -6213,7 +6287,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" s="70" t="s">
         <v>116</v>
       </c>
@@ -6233,7 +6307,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" s="70" t="s">
         <v>116</v>
       </c>
@@ -6251,7 +6325,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" s="70" t="s">
         <v>116</v>
       </c>
@@ -6269,7 +6343,7 @@
       </c>
       <c r="F38" s="77"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" s="70" t="s">
         <v>116</v>
       </c>
@@ -6289,7 +6363,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" s="70" t="s">
         <v>116</v>
       </c>
@@ -6305,7 +6379,7 @@
       <c r="E40" s="70"/>
       <c r="F40" s="77"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" s="71" t="s">
         <v>116</v>
       </c>
@@ -6323,7 +6397,7 @@
       </c>
       <c r="F41" s="76"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" s="70" t="s">
         <v>116</v>
       </c>
@@ -6341,7 +6415,7 @@
       </c>
       <c r="F42" s="77"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" s="71" t="s">
         <v>116</v>
       </c>
@@ -6359,7 +6433,7 @@
       </c>
       <c r="F43" s="76"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" s="71" t="s">
         <v>116</v>
       </c>
@@ -6377,7 +6451,7 @@
       </c>
       <c r="F44" s="76"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" s="70" t="s">
         <v>312</v>
       </c>
@@ -6395,7 +6469,7 @@
       </c>
       <c r="F45" s="77"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" s="70" t="s">
         <v>312</v>
       </c>
@@ -6415,7 +6489,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" s="70" t="s">
         <v>312</v>
       </c>
@@ -6431,7 +6505,7 @@
       <c r="E47" s="70"/>
       <c r="F47" s="77"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" s="70" t="s">
         <v>312</v>
       </c>
@@ -6449,7 +6523,7 @@
       </c>
       <c r="F48" s="77"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" s="70" t="s">
         <v>312</v>
       </c>
@@ -6469,7 +6543,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" s="70" t="s">
         <v>312</v>
       </c>
@@ -6485,7 +6559,7 @@
       <c r="E50" s="70"/>
       <c r="F50" s="77"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" s="70" t="s">
         <v>42</v>
       </c>
@@ -6505,7 +6579,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" s="70" t="s">
         <v>42</v>
       </c>
@@ -6525,7 +6599,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53" s="70" t="s">
         <v>42</v>
       </c>
@@ -6543,7 +6617,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" s="70" t="s">
         <v>42</v>
       </c>
@@ -6561,7 +6635,7 @@
       </c>
       <c r="F54" s="77"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" s="70" t="s">
         <v>42</v>
       </c>
@@ -6581,7 +6655,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" s="70" t="s">
         <v>42</v>
       </c>
@@ -6597,7 +6671,7 @@
       <c r="E56" s="70"/>
       <c r="F56" s="77"/>
     </row>
-    <row r="57" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="70" t="s">
         <v>69</v>
       </c>
@@ -6617,7 +6691,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" ht="13.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="70" t="s">
         <v>69</v>
       </c>
@@ -6637,7 +6711,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" s="70" t="s">
         <v>69</v>
       </c>
@@ -6655,7 +6729,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" s="70" t="s">
         <v>69</v>
       </c>
@@ -6673,7 +6747,7 @@
       </c>
       <c r="F60" s="77"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" s="70" t="s">
         <v>69</v>
       </c>
@@ -6693,7 +6767,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" s="70" t="s">
         <v>69</v>
       </c>
@@ -6709,7 +6783,7 @@
       <c r="E62" s="70"/>
       <c r="F62" s="77"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" s="71" t="s">
         <v>69</v>
       </c>
@@ -6729,7 +6803,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" s="70" t="s">
         <v>64</v>
       </c>
@@ -6747,7 +6821,7 @@
       </c>
       <c r="F64" s="77"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" s="70" t="s">
         <v>64</v>
       </c>
@@ -6767,7 +6841,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" s="70" t="s">
         <v>64</v>
       </c>
@@ -6783,7 +6857,7 @@
       <c r="E66" s="70"/>
       <c r="F66" s="77"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" s="70" t="s">
         <v>64</v>
       </c>
@@ -6801,7 +6875,7 @@
       </c>
       <c r="F67" s="77"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" s="70" t="s">
         <v>64</v>
       </c>
@@ -6821,7 +6895,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" s="70" t="s">
         <v>64</v>
       </c>
@@ -6837,7 +6911,7 @@
       <c r="E69" s="70"/>
       <c r="F69" s="77"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" s="70" t="s">
         <v>10</v>
       </c>
@@ -6855,7 +6929,7 @@
       </c>
       <c r="F70" s="77"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" s="70" t="s">
         <v>10</v>
       </c>
@@ -6873,7 +6947,7 @@
       </c>
       <c r="F71" s="77"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" s="70" t="s">
         <v>10</v>
       </c>
@@ -6889,7 +6963,7 @@
       <c r="E72" s="70"/>
       <c r="F72" s="77"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" s="70" t="s">
         <v>10</v>
       </c>
@@ -6907,7 +6981,7 @@
       </c>
       <c r="F73" s="77"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" s="70" t="s">
         <v>10</v>
       </c>
@@ -6927,7 +7001,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" s="70" t="s">
         <v>10</v>
       </c>
@@ -6943,7 +7017,7 @@
       <c r="E75" s="70"/>
       <c r="F75" s="77"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" s="70" t="s">
         <v>239</v>
       </c>
@@ -6963,7 +7037,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" s="70" t="s">
         <v>239</v>
       </c>
@@ -6981,7 +7055,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" s="70" t="s">
         <v>239</v>
       </c>
@@ -6999,7 +7073,7 @@
       </c>
       <c r="F78" s="77"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" s="70" t="s">
         <v>239</v>
       </c>
@@ -7017,7 +7091,7 @@
       </c>
       <c r="F79" s="77"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" s="70" t="s">
         <v>107</v>
       </c>
@@ -7035,7 +7109,7 @@
       </c>
       <c r="F80" s="77"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" s="70" t="s">
         <v>107</v>
       </c>
@@ -7053,7 +7127,7 @@
       </c>
       <c r="F81" s="77"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" s="70" t="s">
         <v>107</v>
       </c>
@@ -7069,7 +7143,7 @@
       <c r="E82" s="70"/>
       <c r="F82" s="77"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" s="70" t="s">
         <v>107</v>
       </c>
@@ -7087,7 +7161,7 @@
       </c>
       <c r="F83" s="77"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" s="70" t="s">
         <v>107</v>
       </c>
@@ -7107,7 +7181,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" s="70" t="s">
         <v>107</v>
       </c>
@@ -7123,7 +7197,7 @@
       <c r="E85" s="70"/>
       <c r="F85" s="77"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" s="70" t="s">
         <v>363</v>
       </c>
@@ -7143,7 +7217,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" s="70" t="s">
         <v>363</v>
       </c>
@@ -7163,7 +7237,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" s="70" t="s">
         <v>363</v>
       </c>
@@ -7179,7 +7253,7 @@
       <c r="E88" s="70"/>
       <c r="F88" s="77"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" s="70" t="s">
         <v>363</v>
       </c>
@@ -7197,7 +7271,7 @@
       </c>
       <c r="F89" s="77"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" s="70" t="s">
         <v>363</v>
       </c>
@@ -7217,7 +7291,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" s="70" t="s">
         <v>363</v>
       </c>
@@ -7233,7 +7307,7 @@
       <c r="E91" s="70"/>
       <c r="F91" s="77"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" s="70" t="s">
         <v>363</v>
       </c>
@@ -7251,7 +7325,7 @@
       </c>
       <c r="F92" s="77"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" s="70" t="s">
         <v>363</v>
       </c>
@@ -7269,7 +7343,7 @@
       </c>
       <c r="F93" s="77"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" s="70" t="s">
         <v>151</v>
       </c>
@@ -7289,7 +7363,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95" s="70" t="s">
         <v>151</v>
       </c>
@@ -7309,7 +7383,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" s="70" t="s">
         <v>151</v>
       </c>
@@ -7327,7 +7401,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" s="70" t="s">
         <v>151</v>
       </c>
@@ -7345,7 +7419,7 @@
       </c>
       <c r="F97" s="77"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" s="70" t="s">
         <v>151</v>
       </c>
@@ -7365,7 +7439,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" s="70" t="s">
         <v>151</v>
       </c>
@@ -7381,7 +7455,7 @@
       <c r="E99" s="70"/>
       <c r="F99" s="77"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A100" s="70" t="s">
         <v>151</v>
       </c>
@@ -7399,7 +7473,7 @@
       </c>
       <c r="F100" s="77"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" s="70" t="s">
         <v>135</v>
       </c>
@@ -7417,7 +7491,7 @@
       </c>
       <c r="F101" s="77"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" s="70" t="s">
         <v>135</v>
       </c>
@@ -7437,7 +7511,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A103" s="70" t="s">
         <v>135</v>
       </c>
@@ -7453,7 +7527,7 @@
       <c r="E103" s="70"/>
       <c r="F103" s="77"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" s="70" t="s">
         <v>135</v>
       </c>
@@ -7471,7 +7545,7 @@
       </c>
       <c r="F104" s="77"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A105" s="70" t="s">
         <v>135</v>
       </c>
@@ -7489,7 +7563,7 @@
       </c>
       <c r="F105" s="77"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" s="70" t="s">
         <v>135</v>
       </c>
@@ -7509,7 +7583,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" s="70" t="s">
         <v>135</v>
       </c>
@@ -7525,7 +7599,7 @@
       <c r="E107" s="70"/>
       <c r="F107" s="77"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" s="70" t="s">
         <v>17</v>
       </c>
@@ -7543,7 +7617,7 @@
       </c>
       <c r="F108" s="77"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" s="70" t="s">
         <v>17</v>
       </c>
@@ -7563,7 +7637,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" s="70" t="s">
         <v>17</v>
       </c>
@@ -7579,7 +7653,7 @@
       <c r="E110" s="70"/>
       <c r="F110" s="77"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" s="70" t="s">
         <v>17</v>
       </c>
@@ -7597,7 +7671,7 @@
       </c>
       <c r="F111" s="77"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" s="70" t="s">
         <v>17</v>
       </c>
@@ -7617,7 +7691,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A113" s="70" t="s">
         <v>17</v>
       </c>
@@ -7633,7 +7707,7 @@
       <c r="E113" s="70"/>
       <c r="F113" s="77"/>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A114" s="70" t="s">
         <v>93</v>
       </c>
@@ -7650,11 +7724,11 @@
         <v>93</v>
       </c>
       <c r="F114" s="77"/>
-      <c r="G114" s="89" t="s">
+      <c r="G114" s="82" t="s">
         <v>448</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A115" s="70" t="s">
         <v>93</v>
       </c>
@@ -7673,11 +7747,11 @@
       <c r="F115" s="77" t="s">
         <v>407</v>
       </c>
-      <c r="G115" s="90" t="s">
+      <c r="G115" s="83" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A116" s="70" t="s">
         <v>93</v>
       </c>
@@ -7692,11 +7766,11 @@
       </c>
       <c r="E116" s="70"/>
       <c r="F116" s="77"/>
-      <c r="G116" s="90" t="s">
+      <c r="G116" s="83" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A117" s="70" t="s">
         <v>93</v>
       </c>
@@ -7716,7 +7790,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A118" s="70" t="s">
         <v>93</v>
       </c>
@@ -7732,7 +7806,7 @@
       <c r="E118" s="70"/>
       <c r="F118" s="77"/>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A119" s="70" t="s">
         <v>93</v>
       </c>
@@ -7750,7 +7824,7 @@
       </c>
       <c r="F119" s="77"/>
     </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A120" s="70" t="s">
         <v>256</v>
       </c>
@@ -7770,7 +7844,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A121" s="70" t="s">
         <v>256</v>
       </c>
@@ -7790,7 +7864,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A122" s="70" t="s">
         <v>256</v>
       </c>
@@ -7808,7 +7882,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A123" s="70" t="s">
         <v>256</v>
       </c>
@@ -7826,7 +7900,7 @@
       </c>
       <c r="F123" s="77"/>
     </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A124" s="70" t="s">
         <v>256</v>
       </c>
@@ -7846,7 +7920,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A125" s="70" t="s">
         <v>256</v>
       </c>
@@ -7862,7 +7936,7 @@
       <c r="E125" s="70"/>
       <c r="F125" s="77"/>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A126" s="70" t="s">
         <v>103</v>
       </c>
@@ -7882,7 +7956,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A127" s="70" t="s">
         <v>103</v>
       </c>
@@ -7902,7 +7976,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A128" s="70" t="s">
         <v>103</v>
       </c>
@@ -7920,7 +7994,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A129" s="70" t="s">
         <v>103</v>
       </c>
@@ -7938,7 +8012,7 @@
       </c>
       <c r="F129" s="77"/>
     </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A130" s="70" t="s">
         <v>103</v>
       </c>
@@ -7958,7 +8032,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A131" s="70" t="s">
         <v>103</v>
       </c>
@@ -7974,7 +8048,7 @@
       <c r="E131" s="70"/>
       <c r="F131" s="77"/>
     </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A132" s="70" t="s">
         <v>103</v>
       </c>
@@ -7994,68 +8068,68 @@
         <v>407</v>
       </c>
     </row>
-    <row r="133" spans="1:7" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A133" s="109" t="s">
+    <row r="133" spans="1:7" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A133" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="B133" s="110" t="s">
+      <c r="B133" s="92" t="s">
         <v>180</v>
       </c>
-      <c r="C133" s="111" t="s">
+      <c r="C133" s="93" t="s">
         <v>451</v>
       </c>
-      <c r="D133" s="112" t="s">
+      <c r="D133" s="94" t="s">
         <v>452</v>
       </c>
-      <c r="E133" s="109" t="s">
+      <c r="E133" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="F133" s="113"/>
-    </row>
-    <row r="134" spans="1:7" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A134" s="109" t="s">
+      <c r="F133" s="95"/>
+    </row>
+    <row r="134" spans="1:7" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A134" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="B134" s="110" t="s">
+      <c r="B134" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="C134" s="111" t="s">
+      <c r="C134" s="93" t="s">
         <v>451</v>
       </c>
-      <c r="D134" s="112" t="s">
+      <c r="D134" s="94" t="s">
         <v>453</v>
       </c>
-      <c r="E134" s="109" t="s">
+      <c r="E134" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="F134" s="113" t="s">
+      <c r="F134" s="95" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="135" spans="1:7" s="114" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A135" s="109" t="s">
+    <row r="135" spans="1:7" s="96" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A135" s="91" t="s">
         <v>450</v>
       </c>
-      <c r="B135" s="110" t="s">
+      <c r="B135" s="92" t="s">
         <v>182</v>
       </c>
-      <c r="C135" s="111" t="s">
+      <c r="C135" s="93" t="s">
         <v>451</v>
       </c>
-      <c r="D135" s="112" t="s">
+      <c r="D135" s="94" t="s">
         <v>454</v>
       </c>
-      <c r="E135" s="109"/>
-      <c r="F135" s="113"/>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="109" t="s">
+      <c r="E135" s="91"/>
+      <c r="F135" s="95"/>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A136" s="91" t="s">
         <v>450</v>
       </c>
       <c r="B136" s="62" t="s">
         <v>180</v>
       </c>
-      <c r="C136" s="111" t="s">
+      <c r="C136" s="93" t="s">
         <v>464</v>
       </c>
       <c r="D136" s="65" t="s">
@@ -8066,14 +8140,14 @@
       </c>
       <c r="F136" s="76"/>
     </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="109" t="s">
+    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A137" s="91" t="s">
         <v>450</v>
       </c>
       <c r="B137" s="62" t="s">
         <v>183</v>
       </c>
-      <c r="C137" s="111" t="s">
+      <c r="C137" s="93" t="s">
         <v>464</v>
       </c>
       <c r="D137" s="65" t="s">
@@ -8086,14 +8160,14 @@
         <v>407</v>
       </c>
     </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A138" s="109" t="s">
+    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A138" s="91" t="s">
         <v>450</v>
       </c>
       <c r="B138" s="62" t="s">
         <v>182</v>
       </c>
-      <c r="C138" s="111" t="s">
+      <c r="C138" s="93" t="s">
         <v>464</v>
       </c>
       <c r="D138" s="65" t="s">
@@ -8102,7 +8176,7 @@
       <c r="E138" s="70"/>
       <c r="F138" s="76"/>
     </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A139" s="70" t="s">
         <v>450</v>
       </c>
@@ -8118,7 +8192,7 @@
       <c r="E139" s="70"/>
       <c r="F139" s="76"/>
     </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A140" s="70" t="s">
         <v>450</v>
       </c>
@@ -8136,7 +8210,7 @@
       </c>
       <c r="F140" s="76"/>
     </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A141" s="70" t="s">
         <v>450</v>
       </c>
@@ -8154,7 +8228,7 @@
       </c>
       <c r="F141" s="76"/>
     </row>
-    <row r="142" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A142" s="70" t="s">
         <v>450</v>
       </c>
@@ -8172,7 +8246,7 @@
       </c>
       <c r="F142" s="76"/>
     </row>
-    <row r="143" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A143" s="70" t="s">
         <v>450</v>
       </c>
@@ -8188,7 +8262,7 @@
       <c r="E143" s="70"/>
       <c r="F143" s="76"/>
     </row>
-    <row r="144" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A144" s="70" t="s">
         <v>0</v>
       </c>
@@ -8207,11 +8281,11 @@
       <c r="F144" s="76" t="s">
         <v>406</v>
       </c>
-      <c r="G144" s="90" t="s">
+      <c r="G144" s="83" t="s">
         <v>447</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" s="70" t="s">
         <v>0</v>
       </c>
@@ -8229,7 +8303,7 @@
       </c>
       <c r="F145" s="76"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" s="70" t="s">
         <v>0</v>
       </c>
@@ -8249,7 +8323,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" s="70" t="s">
         <v>0</v>
       </c>
@@ -8265,7 +8339,7 @@
       <c r="E147" s="70"/>
       <c r="F147" s="76"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A148" s="70" t="s">
         <v>0</v>
       </c>
@@ -8285,7 +8359,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" s="70" t="s">
         <v>0</v>
       </c>
@@ -8303,7 +8377,7 @@
       </c>
       <c r="F149" s="76"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" s="70" t="s">
         <v>0</v>
       </c>
@@ -8321,7 +8395,7 @@
       </c>
       <c r="F150" s="76"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" s="70" t="s">
         <v>0</v>
       </c>
@@ -8339,7 +8413,7 @@
       </c>
       <c r="F151" s="76"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" s="70" t="s">
         <v>0</v>
       </c>
@@ -8359,7 +8433,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" s="70" t="s">
         <v>0</v>
       </c>
@@ -8375,7 +8449,7 @@
       <c r="E153" s="70"/>
       <c r="F153" s="76"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" s="70" t="s">
         <v>0</v>
       </c>
@@ -8395,7 +8469,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" s="70" t="s">
         <v>387</v>
       </c>
@@ -8413,7 +8487,7 @@
       </c>
       <c r="F155" s="77"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" s="70" t="s">
         <v>387</v>
       </c>
@@ -8433,7 +8507,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" s="70" t="s">
         <v>387</v>
       </c>
@@ -8449,7 +8523,7 @@
       <c r="E157" s="70"/>
       <c r="F157" s="77"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" s="70" t="s">
         <v>387</v>
       </c>
@@ -8467,7 +8541,7 @@
       </c>
       <c r="F158" s="77"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" s="70" t="s">
         <v>387</v>
       </c>
@@ -8487,7 +8561,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" s="70" t="s">
         <v>387</v>
       </c>
@@ -8503,7 +8577,7 @@
       <c r="E160" s="70"/>
       <c r="F160" s="77"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" s="70" t="s">
         <v>387</v>
       </c>
@@ -8521,95 +8595,95 @@
       </c>
       <c r="F161" s="77"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A162" s="91" t="s">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A162" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B162" s="92" t="s">
+      <c r="B162" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="C162" s="93" t="s">
+      <c r="C162" s="86" t="s">
         <v>401</v>
       </c>
-      <c r="D162" s="94" t="s">
+      <c r="D162" s="87" t="s">
         <v>398</v>
       </c>
-      <c r="E162" s="91" t="s">
+      <c r="E162" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="F162" s="95" t="s">
+      <c r="F162" s="88" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A163" s="91" t="s">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A163" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B163" s="92" t="s">
+      <c r="B163" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="C163" s="93" t="s">
+      <c r="C163" s="86" t="s">
         <v>426</v>
       </c>
-      <c r="D163" s="94" t="s">
+      <c r="D163" s="87" t="s">
         <v>427</v>
       </c>
-      <c r="E163" s="91" t="s">
+      <c r="E163" s="84" t="s">
         <v>0</v>
       </c>
-      <c r="F163" s="95"/>
-    </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A164" s="91" t="s">
+      <c r="F163" s="88"/>
+    </row>
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A164" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B164" s="92" t="s">
+      <c r="B164" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="C164" s="93" t="s">
+      <c r="C164" s="86" t="s">
         <v>402</v>
       </c>
-      <c r="D164" s="94" t="s">
+      <c r="D164" s="87" t="s">
         <v>399</v>
       </c>
-      <c r="E164" s="91" t="s">
+      <c r="E164" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="F164" s="95"/>
-    </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A165" s="91" t="s">
+      <c r="F164" s="88"/>
+    </row>
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A165" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B165" s="92" t="s">
+      <c r="B165" s="85" t="s">
         <v>182</v>
       </c>
-      <c r="C165" s="93" t="s">
+      <c r="C165" s="86" t="s">
         <v>402</v>
       </c>
-      <c r="D165" s="94" t="s">
+      <c r="D165" s="87" t="s">
         <v>400</v>
       </c>
-      <c r="E165" s="91"/>
-      <c r="F165" s="95"/>
-    </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A166" s="91" t="s">
+      <c r="E165" s="84"/>
+      <c r="F165" s="88"/>
+    </row>
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A166" s="84" t="s">
         <v>88</v>
       </c>
-      <c r="B166" s="92" t="s">
+      <c r="B166" s="85" t="s">
         <v>182</v>
       </c>
-      <c r="C166" s="93" t="s">
+      <c r="C166" s="86" t="s">
         <v>403</v>
       </c>
-      <c r="D166" s="94" t="s">
+      <c r="D166" s="87" t="s">
         <v>404</v>
       </c>
-      <c r="E166" s="91"/>
-      <c r="F166" s="95"/>
-    </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E166" s="84"/>
+      <c r="F166" s="88"/>
+    </row>
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" s="70" t="s">
         <v>163</v>
       </c>
@@ -8627,7 +8701,7 @@
       </c>
       <c r="F167" s="77"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" s="70" t="s">
         <v>163</v>
       </c>
@@ -8647,7 +8721,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A169" s="70" t="s">
         <v>163</v>
       </c>
@@ -8663,7 +8737,7 @@
       <c r="E169" s="70"/>
       <c r="F169" s="77"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" s="70" t="s">
         <v>163</v>
       </c>
@@ -8681,7 +8755,7 @@
       </c>
       <c r="F170" s="77"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" s="70" t="s">
         <v>163</v>
       </c>
@@ -8701,7 +8775,7 @@
         <v>407</v>
       </c>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A172" s="70" t="s">
         <v>163</v>
       </c>
@@ -8717,7 +8791,7 @@
       <c r="E172" s="70"/>
       <c r="F172" s="77"/>
     </row>
-    <row r="173" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A173" s="72" t="s">
         <v>163</v>
       </c>
@@ -8740,6 +8814,9 @@
     <sortCondition ref="C133:C143"/>
     <sortCondition ref="B133:B143" customList="GET,PUT,POST,DELETE"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="56" fitToHeight="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
@@ -8747,208 +8824,76 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="A1:E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5703125" customWidth="1"/>
-    <col min="4" max="4" width="19.140625" customWidth="1"/>
-    <col min="5" max="5" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19" style="113" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.88671875" style="113" customWidth="1"/>
+    <col min="3" max="3" width="29" style="113" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="68" t="s">
-        <v>177</v>
-      </c>
-      <c r="B1" s="68" t="s">
-        <v>178</v>
-      </c>
-      <c r="C1" s="68" t="s">
-        <v>179</v>
-      </c>
-      <c r="D1" s="79" t="s">
-        <v>425</v>
-      </c>
-      <c r="E1" s="69" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="83" t="s">
-        <v>180</v>
-      </c>
-      <c r="B2" s="84" t="s">
-        <v>378</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>380</v>
-      </c>
-      <c r="D2" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E2" s="86"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="83" t="s">
-        <v>181</v>
-      </c>
-      <c r="B3" s="84" t="s">
-        <v>378</v>
-      </c>
-      <c r="C3" s="12" t="s">
-        <v>382</v>
-      </c>
-      <c r="D3" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E3" s="86" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="83" t="s">
-        <v>182</v>
-      </c>
-      <c r="B4" s="84" t="s">
-        <v>378</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>381</v>
-      </c>
-      <c r="D4" s="85"/>
-      <c r="E4" s="86"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="83" t="s">
-        <v>180</v>
-      </c>
-      <c r="B5" s="84" t="s">
-        <v>379</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>383</v>
-      </c>
-      <c r="D5" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E5" s="86"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="83" t="s">
-        <v>183</v>
-      </c>
-      <c r="B6" s="84" t="s">
-        <v>379</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>384</v>
-      </c>
-      <c r="D6" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E6" s="86" t="s">
-        <v>407</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="83" t="s">
-        <v>182</v>
-      </c>
-      <c r="B7" s="84" t="s">
-        <v>379</v>
-      </c>
-      <c r="C7" s="12" t="s">
-        <v>385</v>
-      </c>
-      <c r="D7" s="85"/>
-      <c r="E7" s="86"/>
-    </row>
-    <row r="8" spans="1:5" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="83" t="s">
-        <v>180</v>
-      </c>
-      <c r="B8" s="84" t="s">
-        <v>386</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>428</v>
-      </c>
-      <c r="D8" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="86"/>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="12"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="86"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="85"/>
-      <c r="E10" s="86"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="85"/>
-      <c r="E11" s="86"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="12"/>
-      <c r="D12" s="85"/>
-      <c r="E12" s="86"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="83"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="85"/>
-      <c r="E13" s="86"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="85"/>
-      <c r="E14" s="86"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="12"/>
-      <c r="D15" s="85"/>
-      <c r="E15" s="86"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="12"/>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="86"/>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="110" t="s">
+        <v>472</v>
+      </c>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="112" t="s">
+        <v>473</v>
+      </c>
+      <c r="B2" s="112" t="s">
+        <v>474</v>
+      </c>
+      <c r="C2" s="112" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="113" t="s">
+        <v>476</v>
+      </c>
+      <c r="B3" s="113" t="s">
+        <v>478</v>
+      </c>
+      <c r="C3" s="113" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B4" s="113" t="s">
+        <v>480</v>
+      </c>
+      <c r="C4" s="113" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="113" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C14" s="113" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="C15" s="113" t="s">
+        <v>483</v>
+      </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
changes for mailing and texts
</commit_message>
<xml_diff>
--- a/documentation/DataAndAPIMatchAware.xlsx
+++ b/documentation/DataAndAPIMatchAware.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entities" sheetId="1" r:id="rId1"/>
@@ -2599,6 +2599,18 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2607,18 +2619,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2941,7 +2941,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2951,7 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E316"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K292" sqref="K292"/>
     </sheetView>
   </sheetViews>
@@ -2965,13 +2965,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="162" t="s">
+      <c r="A1" s="156" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="162"/>
-      <c r="C1" s="162"/>
-      <c r="D1" s="162"/>
-      <c r="E1" s="162"/>
+      <c r="B1" s="156"/>
+      <c r="C1" s="156"/>
+      <c r="D1" s="156"/>
+      <c r="E1" s="156"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="88"/>
@@ -2981,13 +2981,13 @@
       <c r="E2" s="88"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="159" t="s">
+      <c r="A3" s="157" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="160"/>
-      <c r="C3" s="160"/>
-      <c r="D3" s="160"/>
-      <c r="E3" s="161"/>
+      <c r="B3" s="158"/>
+      <c r="C3" s="158"/>
+      <c r="D3" s="158"/>
+      <c r="E3" s="159"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -3112,13 +3112,13 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="159" t="s">
+      <c r="A14" s="157" t="s">
         <v>290</v>
       </c>
-      <c r="B14" s="160"/>
-      <c r="C14" s="160"/>
-      <c r="D14" s="160"/>
-      <c r="E14" s="161"/>
+      <c r="B14" s="158"/>
+      <c r="C14" s="158"/>
+      <c r="D14" s="158"/>
+      <c r="E14" s="159"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
@@ -3195,13 +3195,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="159" t="s">
+      <c r="A21" s="157" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="160"/>
-      <c r="C21" s="160"/>
-      <c r="D21" s="160"/>
-      <c r="E21" s="161"/>
+      <c r="B21" s="158"/>
+      <c r="C21" s="158"/>
+      <c r="D21" s="158"/>
+      <c r="E21" s="159"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
@@ -3274,13 +3274,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="159" t="s">
+      <c r="A28" s="157" t="s">
         <v>279</v>
       </c>
-      <c r="B28" s="160"/>
-      <c r="C28" s="160"/>
-      <c r="D28" s="160"/>
-      <c r="E28" s="161"/>
+      <c r="B28" s="158"/>
+      <c r="C28" s="158"/>
+      <c r="D28" s="158"/>
+      <c r="E28" s="159"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
@@ -3675,13 +3675,13 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="159" t="s">
+      <c r="A61" s="157" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="160"/>
-      <c r="C61" s="160"/>
-      <c r="D61" s="160"/>
-      <c r="E61" s="161"/>
+      <c r="B61" s="158"/>
+      <c r="C61" s="158"/>
+      <c r="D61" s="158"/>
+      <c r="E61" s="159"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14" t="s">
@@ -4015,13 +4015,13 @@
     </row>
     <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="159" t="s">
+      <c r="A89" s="157" t="s">
         <v>96</v>
       </c>
-      <c r="B89" s="160"/>
-      <c r="C89" s="160"/>
-      <c r="D89" s="160"/>
-      <c r="E89" s="161"/>
+      <c r="B89" s="158"/>
+      <c r="C89" s="158"/>
+      <c r="D89" s="158"/>
+      <c r="E89" s="159"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
@@ -5296,13 +5296,13 @@
     </row>
     <row r="197" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="198" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="159" t="s">
+      <c r="A198" s="157" t="s">
         <v>123</v>
       </c>
-      <c r="B198" s="160"/>
-      <c r="C198" s="160"/>
-      <c r="D198" s="160"/>
-      <c r="E198" s="161"/>
+      <c r="B198" s="158"/>
+      <c r="C198" s="158"/>
+      <c r="D198" s="158"/>
+      <c r="E198" s="159"/>
     </row>
     <row r="199" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
@@ -5375,13 +5375,13 @@
     </row>
     <row r="204" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="205" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="159" t="s">
+      <c r="A205" s="157" t="s">
         <v>134</v>
       </c>
-      <c r="B205" s="160"/>
-      <c r="C205" s="160"/>
-      <c r="D205" s="160"/>
-      <c r="E205" s="161"/>
+      <c r="B205" s="158"/>
+      <c r="C205" s="158"/>
+      <c r="D205" s="158"/>
+      <c r="E205" s="159"/>
     </row>
     <row r="206" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
@@ -5476,13 +5476,13 @@
     </row>
     <row r="213" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="214" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="159" t="s">
+      <c r="A214" s="157" t="s">
         <v>285</v>
       </c>
-      <c r="B214" s="160"/>
-      <c r="C214" s="160"/>
-      <c r="D214" s="160"/>
-      <c r="E214" s="161"/>
+      <c r="B214" s="158"/>
+      <c r="C214" s="158"/>
+      <c r="D214" s="158"/>
+      <c r="E214" s="159"/>
     </row>
     <row r="215" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="14" t="s">
@@ -5712,13 +5712,13 @@
     </row>
     <row r="233" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="234" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="156" t="s">
+      <c r="A234" s="160" t="s">
         <v>287</v>
       </c>
-      <c r="B234" s="157"/>
-      <c r="C234" s="157"/>
-      <c r="D234" s="157"/>
-      <c r="E234" s="158"/>
+      <c r="B234" s="161"/>
+      <c r="C234" s="161"/>
+      <c r="D234" s="161"/>
+      <c r="E234" s="162"/>
     </row>
     <row r="235" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="14" t="s">
@@ -6289,13 +6289,13 @@
     </row>
     <row r="282" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="283" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="159" t="s">
+      <c r="A283" s="157" t="s">
         <v>289</v>
       </c>
-      <c r="B283" s="160"/>
-      <c r="C283" s="160"/>
-      <c r="D283" s="160"/>
-      <c r="E283" s="161"/>
+      <c r="B283" s="158"/>
+      <c r="C283" s="158"/>
+      <c r="D283" s="158"/>
+      <c r="E283" s="159"/>
     </row>
     <row r="284" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="30" t="s">
@@ -6708,6 +6708,28 @@
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A303:E303"/>
+    <mergeCell ref="A312:E312"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="A248:E248"/>
+    <mergeCell ref="A269:E269"/>
+    <mergeCell ref="A277:E277"/>
+    <mergeCell ref="A283:E283"/>
+    <mergeCell ref="A193:E193"/>
+    <mergeCell ref="A198:E198"/>
+    <mergeCell ref="A205:E205"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A225:E225"/>
+    <mergeCell ref="A140:E140"/>
+    <mergeCell ref="A157:E157"/>
+    <mergeCell ref="A167:E167"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="A94:E94"/>
+    <mergeCell ref="A125:E125"/>
     <mergeCell ref="A46:E46"/>
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="A14:E14"/>
@@ -6715,28 +6737,6 @@
     <mergeCell ref="A28:E28"/>
     <mergeCell ref="A38:E38"/>
     <mergeCell ref="A3:E3"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="A94:E94"/>
-    <mergeCell ref="A125:E125"/>
-    <mergeCell ref="A140:E140"/>
-    <mergeCell ref="A157:E157"/>
-    <mergeCell ref="A167:E167"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A193:E193"/>
-    <mergeCell ref="A198:E198"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A214:E214"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A303:E303"/>
-    <mergeCell ref="A312:E312"/>
-    <mergeCell ref="A234:E234"/>
-    <mergeCell ref="A248:E248"/>
-    <mergeCell ref="A269:E269"/>
-    <mergeCell ref="A277:E277"/>
-    <mergeCell ref="A283:E283"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6750,7 +6750,7 @@
   </sheetPr>
   <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="A156" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="H45" sqref="A38:H45"/>
     </sheetView>
   </sheetViews>
@@ -11171,7 +11171,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
updates for new path
</commit_message>
<xml_diff>
--- a/documentation/DataAndAPIMatchAware.xlsx
+++ b/documentation/DataAndAPIMatchAware.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16215" windowHeight="9060" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data Entities" sheetId="1" r:id="rId1"/>
@@ -836,9 +836,6 @@
     <t>Delete all user invites</t>
   </si>
   <si>
-    <t>Create user invites</t>
-  </si>
-  <si>
     <t>Retrieve invite by key</t>
   </si>
   <si>
@@ -1647,6 +1644,9 @@
   </si>
   <si>
     <t xml:space="preserve">Replaces all current roles with those provided in the body </t>
+  </si>
+  <si>
+    <t>Create user invites and send email</t>
   </si>
 </sst>
 </file>
@@ -2599,26 +2599,26 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2941,7 +2941,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2951,7 +2951,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E316"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="K292" sqref="K292"/>
     </sheetView>
   </sheetViews>
@@ -2965,13 +2965,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="21" x14ac:dyDescent="0.25">
-      <c r="A1" s="156" t="s">
+      <c r="A1" s="162" t="s">
         <v>37</v>
       </c>
-      <c r="B1" s="156"/>
-      <c r="C1" s="156"/>
-      <c r="D1" s="156"/>
-      <c r="E1" s="156"/>
+      <c r="B1" s="162"/>
+      <c r="C1" s="162"/>
+      <c r="D1" s="162"/>
+      <c r="E1" s="162"/>
     </row>
     <row r="2" spans="1:5" ht="21.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="88"/>
@@ -2981,13 +2981,13 @@
       <c r="E2" s="88"/>
     </row>
     <row r="3" spans="1:5" s="1" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="157" t="s">
+      <c r="A3" s="159" t="s">
         <v>92</v>
       </c>
-      <c r="B3" s="158"/>
-      <c r="C3" s="158"/>
-      <c r="D3" s="158"/>
-      <c r="E3" s="159"/>
+      <c r="B3" s="160"/>
+      <c r="C3" s="160"/>
+      <c r="D3" s="160"/>
+      <c r="E3" s="161"/>
     </row>
     <row r="4" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="14" t="s">
@@ -3112,13 +3112,13 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="157" t="s">
-        <v>290</v>
-      </c>
-      <c r="B14" s="158"/>
-      <c r="C14" s="158"/>
-      <c r="D14" s="158"/>
-      <c r="E14" s="159"/>
+      <c r="A14" s="159" t="s">
+        <v>289</v>
+      </c>
+      <c r="B14" s="160"/>
+      <c r="C14" s="160"/>
+      <c r="D14" s="160"/>
+      <c r="E14" s="161"/>
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="14" t="s">
@@ -3195,13 +3195,13 @@
     </row>
     <row r="20" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="157" t="s">
+      <c r="A21" s="159" t="s">
         <v>121</v>
       </c>
-      <c r="B21" s="158"/>
-      <c r="C21" s="158"/>
-      <c r="D21" s="158"/>
-      <c r="E21" s="159"/>
+      <c r="B21" s="160"/>
+      <c r="C21" s="160"/>
+      <c r="D21" s="160"/>
+      <c r="E21" s="161"/>
     </row>
     <row r="22" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="14" t="s">
@@ -3252,7 +3252,7 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B25" s="5" t="s">
         <v>3</v>
@@ -3263,7 +3263,7 @@
     </row>
     <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B26" s="11" t="s">
         <v>3</v>
@@ -3274,13 +3274,13 @@
     </row>
     <row r="27" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="157" t="s">
-        <v>279</v>
-      </c>
-      <c r="B28" s="158"/>
-      <c r="C28" s="158"/>
-      <c r="D28" s="158"/>
-      <c r="E28" s="159"/>
+      <c r="A28" s="159" t="s">
+        <v>278</v>
+      </c>
+      <c r="B28" s="160"/>
+      <c r="C28" s="160"/>
+      <c r="D28" s="160"/>
+      <c r="E28" s="161"/>
     </row>
     <row r="29" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="14" t="s">
@@ -3395,7 +3395,7 @@
     <row r="37" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="153" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B38" s="154"/>
       <c r="C38" s="154"/>
@@ -3447,37 +3447,37 @@
         <v>5</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E41" s="21"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
+        <v>360</v>
+      </c>
+      <c r="B42" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C42" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="B42" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C42" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D42" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="E42" s="21"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="32" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C43" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E43" s="21"/>
     </row>
@@ -3495,7 +3495,7 @@
     <row r="45" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="46" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="153" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B46" s="154"/>
       <c r="C46" s="154"/>
@@ -3566,21 +3566,21 @@
     </row>
     <row r="51" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B51" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C51" s="33"/>
       <c r="D51" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E51" s="34"/>
     </row>
     <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="53" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A53" s="153" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B53" s="154"/>
       <c r="C53" s="154"/>
@@ -3623,7 +3623,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>20</v>
@@ -3649,7 +3649,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>20</v>
@@ -3662,7 +3662,7 @@
     </row>
     <row r="59" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B59" s="35" t="s">
         <v>20</v>
@@ -3675,13 +3675,13 @@
     </row>
     <row r="60" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="61" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="157" t="s">
+      <c r="A61" s="159" t="s">
         <v>97</v>
       </c>
-      <c r="B61" s="158"/>
-      <c r="C61" s="158"/>
-      <c r="D61" s="158"/>
-      <c r="E61" s="159"/>
+      <c r="B61" s="160"/>
+      <c r="C61" s="160"/>
+      <c r="D61" s="160"/>
+      <c r="E61" s="161"/>
     </row>
     <row r="62" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" s="14" t="s">
@@ -3743,14 +3743,14 @@
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B66" s="5" t="s">
         <v>20</v>
       </c>
       <c r="C66" s="18"/>
       <c r="D66" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E66" s="21"/>
     </row>
@@ -3842,13 +3842,13 @@
       </c>
       <c r="C74" s="18"/>
       <c r="D74" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E74" s="21"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B75" s="5" t="s">
         <v>3</v>
@@ -3861,7 +3861,7 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B76" s="5" t="s">
         <v>3</v>
@@ -3874,7 +3874,7 @@
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B77" s="5" t="s">
         <v>3</v>
@@ -3887,27 +3887,27 @@
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B78" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C78" s="18"/>
       <c r="D78" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E78" s="21"/>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B79" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C79" s="18"/>
       <c r="D79" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E79" s="21"/>
     </row>
@@ -3922,7 +3922,7 @@
         <v>5</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E80" s="21"/>
     </row>
@@ -3937,7 +3937,7 @@
         <v>5</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E81" s="21"/>
     </row>
@@ -3978,14 +3978,14 @@
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="48" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B85" s="44" t="s">
         <v>20</v>
       </c>
       <c r="C85" s="45"/>
       <c r="D85" s="44" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E85" s="49"/>
     </row>
@@ -4015,13 +4015,13 @@
     </row>
     <row r="88" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="89" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="157" t="s">
+      <c r="A89" s="159" t="s">
         <v>96</v>
       </c>
-      <c r="B89" s="158"/>
-      <c r="C89" s="158"/>
-      <c r="D89" s="158"/>
-      <c r="E89" s="159"/>
+      <c r="B89" s="160"/>
+      <c r="C89" s="160"/>
+      <c r="D89" s="160"/>
+      <c r="E89" s="161"/>
     </row>
     <row r="90" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A90" s="14" t="s">
@@ -4075,7 +4075,7 @@
     <row r="93" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="94" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="153" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B94" s="154"/>
       <c r="C94" s="154"/>
@@ -4159,7 +4159,7 @@
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="32" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B100" s="5" t="s">
         <v>118</v>
@@ -4222,10 +4222,10 @@
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="32" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B105" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C105" s="5"/>
       <c r="D105" s="5"/>
@@ -4233,10 +4233,10 @@
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="32" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B106" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C106" s="5"/>
       <c r="D106" s="5"/>
@@ -4409,7 +4409,7 @@
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" s="32" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B122" s="8" t="s">
         <v>3</v>
@@ -4420,7 +4420,7 @@
     </row>
     <row r="123" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="80" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B123" s="35" t="s">
         <v>118</v>
@@ -4432,7 +4432,7 @@
     <row r="124" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="125" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A125" s="153" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B125" s="154"/>
       <c r="C125" s="154"/>
@@ -4530,7 +4530,7 @@
         <v>66</v>
       </c>
       <c r="B132" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C132" s="5"/>
       <c r="D132" s="5"/>
@@ -4571,7 +4571,7 @@
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B136" s="5" t="s">
         <v>26</v>
@@ -4595,7 +4595,7 @@
     </row>
     <row r="138" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="80" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B138" s="35" t="s">
         <v>118</v>
@@ -4607,7 +4607,7 @@
     <row r="139" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="140" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="153" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B140" s="154"/>
       <c r="C140" s="154"/>
@@ -4694,7 +4694,7 @@
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" s="7" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B147" s="5" t="s">
         <v>26</v>
@@ -4705,37 +4705,37 @@
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="B148" s="5" t="s">
+        <v>302</v>
+      </c>
+      <c r="C148" s="18" t="s">
+        <v>5</v>
+      </c>
+      <c r="D148" s="5" t="s">
         <v>361</v>
-      </c>
-      <c r="B148" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="C148" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="D148" s="5" t="s">
-        <v>362</v>
       </c>
       <c r="E148" s="21"/>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" s="7" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B149" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C149" s="18" t="s">
         <v>5</v>
       </c>
       <c r="D149" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E149" s="21"/>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" s="7" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B150" s="5" t="s">
         <v>3</v>
@@ -4746,7 +4746,7 @@
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" s="7" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B151" s="5" t="s">
         <v>3</v>
@@ -4757,7 +4757,7 @@
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" s="7" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B152" s="5" t="s">
         <v>3</v>
@@ -4775,7 +4775,7 @@
       </c>
       <c r="C153" s="18"/>
       <c r="D153" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E153" s="21"/>
     </row>
@@ -4788,27 +4788,27 @@
       </c>
       <c r="C154" s="18"/>
       <c r="D154" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E154" s="21"/>
     </row>
     <row r="155" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A155" s="10" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B155" s="11" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C155" s="11"/>
       <c r="D155" s="11" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E155" s="12"/>
     </row>
     <row r="156" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="157" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A157" s="153" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B157" s="154"/>
       <c r="C157" s="154"/>
@@ -4910,21 +4910,21 @@
     </row>
     <row r="165" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A165" s="80" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B165" s="35" t="s">
         <v>3</v>
       </c>
       <c r="C165" s="59"/>
       <c r="D165" s="86" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E165" s="47"/>
     </row>
     <row r="166" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="167" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A167" s="153" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B167" s="154"/>
       <c r="C167" s="154"/>
@@ -4983,7 +4983,7 @@
         <v>130</v>
       </c>
       <c r="B171" s="11" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C171" s="33"/>
       <c r="D171" s="11"/>
@@ -4998,7 +4998,7 @@
     </row>
     <row r="173" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A173" s="153" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="B173" s="154"/>
       <c r="C173" s="154"/>
@@ -5104,53 +5104,53 @@
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="7" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B181" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C181" s="18"/>
       <c r="D181" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E181" s="21"/>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="32" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B182" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C182" s="51"/>
       <c r="D182" s="51" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E182" s="46"/>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="32" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B183" s="8" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C183" s="51"/>
       <c r="D183" s="51" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E183" s="46"/>
     </row>
     <row r="184" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A184" s="10" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B184" s="11" t="s">
         <v>3</v>
       </c>
       <c r="C184" s="33"/>
       <c r="D184" s="11" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E184" s="34"/>
     </row>
@@ -5226,7 +5226,7 @@
     </row>
     <row r="191" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A191" s="10" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B191" s="35" t="s">
         <v>20</v>
@@ -5238,7 +5238,7 @@
     <row r="192" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="193" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A193" s="153" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="B193" s="154"/>
       <c r="C193" s="154"/>
@@ -5296,13 +5296,13 @@
     </row>
     <row r="197" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="198" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A198" s="157" t="s">
+      <c r="A198" s="159" t="s">
         <v>123</v>
       </c>
-      <c r="B198" s="158"/>
-      <c r="C198" s="158"/>
-      <c r="D198" s="158"/>
-      <c r="E198" s="159"/>
+      <c r="B198" s="160"/>
+      <c r="C198" s="160"/>
+      <c r="D198" s="160"/>
+      <c r="E198" s="161"/>
     </row>
     <row r="199" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A199" s="14" t="s">
@@ -5353,7 +5353,7 @@
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" s="7" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B202" s="5" t="s">
         <v>3</v>
@@ -5364,7 +5364,7 @@
     </row>
     <row r="203" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A203" s="10" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B203" s="11" t="s">
         <v>3</v>
@@ -5375,13 +5375,13 @@
     </row>
     <row r="204" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="205" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A205" s="157" t="s">
+      <c r="A205" s="159" t="s">
         <v>134</v>
       </c>
-      <c r="B205" s="158"/>
-      <c r="C205" s="158"/>
-      <c r="D205" s="158"/>
-      <c r="E205" s="159"/>
+      <c r="B205" s="160"/>
+      <c r="C205" s="160"/>
+      <c r="D205" s="160"/>
+      <c r="E205" s="161"/>
     </row>
     <row r="206" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A206" s="14" t="s">
@@ -5463,26 +5463,26 @@
     </row>
     <row r="212" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A212" s="80" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B212" s="35" t="s">
         <v>6</v>
       </c>
       <c r="C212" s="59"/>
       <c r="D212" s="87" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E212" s="47"/>
     </row>
     <row r="213" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="214" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A214" s="157" t="s">
-        <v>285</v>
-      </c>
-      <c r="B214" s="158"/>
-      <c r="C214" s="158"/>
-      <c r="D214" s="158"/>
-      <c r="E214" s="159"/>
+      <c r="A214" s="159" t="s">
+        <v>284</v>
+      </c>
+      <c r="B214" s="160"/>
+      <c r="C214" s="160"/>
+      <c r="D214" s="160"/>
+      <c r="E214" s="161"/>
     </row>
     <row r="215" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A215" s="14" t="s">
@@ -5550,14 +5550,14 @@
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" s="7" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B219" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C219" s="18"/>
       <c r="D219" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="E219" s="21"/>
     </row>
@@ -5608,7 +5608,7 @@
     <row r="224" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="225" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A225" s="153" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B225" s="154"/>
       <c r="C225" s="154"/>
@@ -5712,13 +5712,13 @@
     </row>
     <row r="233" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="234" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A234" s="160" t="s">
-        <v>287</v>
-      </c>
-      <c r="B234" s="161"/>
-      <c r="C234" s="161"/>
-      <c r="D234" s="161"/>
-      <c r="E234" s="162"/>
+      <c r="A234" s="156" t="s">
+        <v>286</v>
+      </c>
+      <c r="B234" s="157"/>
+      <c r="C234" s="157"/>
+      <c r="D234" s="157"/>
+      <c r="E234" s="158"/>
     </row>
     <row r="235" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A235" s="14" t="s">
@@ -5830,7 +5830,7 @@
       <c r="B244" s="5"/>
       <c r="C244" s="5"/>
       <c r="D244" s="27" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="E244" s="6"/>
     </row>
@@ -5839,13 +5839,13 @@
       <c r="B245" s="5"/>
       <c r="C245" s="5"/>
       <c r="D245" s="27" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="E245" s="6"/>
     </row>
     <row r="246" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A246" s="10" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B246" s="35" t="s">
         <v>20</v>
@@ -5931,7 +5931,7 @@
         <v>18</v>
       </c>
       <c r="B253" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C253" s="18"/>
       <c r="D253" s="82">
@@ -5944,7 +5944,7 @@
         <v>24</v>
       </c>
       <c r="B254" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C254" s="18"/>
       <c r="D254" s="82">
@@ -5954,10 +5954,10 @@
     </row>
     <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" s="7" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B255" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C255" s="18"/>
       <c r="D255" s="82">
@@ -5974,7 +5974,7 @@
       </c>
       <c r="C256" s="18"/>
       <c r="D256" s="83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E256" s="6"/>
     </row>
@@ -5983,7 +5983,7 @@
         <v>27</v>
       </c>
       <c r="B257" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C257" s="18"/>
       <c r="D257" s="82">
@@ -5996,7 +5996,7 @@
         <v>28</v>
       </c>
       <c r="B258" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C258" s="18"/>
       <c r="D258" s="82">
@@ -6009,7 +6009,7 @@
         <v>29</v>
       </c>
       <c r="B259" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C259" s="18"/>
       <c r="D259" s="82">
@@ -6022,7 +6022,7 @@
         <v>30</v>
       </c>
       <c r="B260" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C260" s="18"/>
       <c r="D260" s="82">
@@ -6035,7 +6035,7 @@
         <v>31</v>
       </c>
       <c r="B261" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C261" s="18"/>
       <c r="D261" s="82">
@@ -6048,7 +6048,7 @@
         <v>32</v>
       </c>
       <c r="B262" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C262" s="18"/>
       <c r="D262" s="82">
@@ -6058,10 +6058,10 @@
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" s="7" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B263" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C263" s="18"/>
       <c r="D263" s="82">
@@ -6078,7 +6078,7 @@
       </c>
       <c r="C264" s="18"/>
       <c r="D264" s="82" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E264" s="6"/>
     </row>
@@ -6091,7 +6091,7 @@
       </c>
       <c r="C265" s="18"/>
       <c r="D265" s="83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E265" s="6"/>
     </row>
@@ -6104,7 +6104,7 @@
       </c>
       <c r="C266" s="18"/>
       <c r="D266" s="83" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E266" s="6"/>
     </row>
@@ -6117,7 +6117,7 @@
       </c>
       <c r="C267" s="19"/>
       <c r="D267" s="85" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E267" s="12"/>
     </row>
@@ -6130,7 +6130,7 @@
     </row>
     <row r="269" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A269" s="153" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B269" s="154"/>
       <c r="C269" s="154"/>
@@ -6186,7 +6186,7 @@
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" s="7" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B273" s="5" t="s">
         <v>20</v>
@@ -6224,7 +6224,7 @@
     <row r="276" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="277" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A277" s="153" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B277" s="154"/>
       <c r="C277" s="154"/>
@@ -6263,7 +6263,7 @@
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" s="7" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B280" s="5" t="s">
         <v>20</v>
@@ -6289,13 +6289,13 @@
     </row>
     <row r="282" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="283" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A283" s="157" t="s">
-        <v>289</v>
-      </c>
-      <c r="B283" s="158"/>
-      <c r="C283" s="158"/>
-      <c r="D283" s="158"/>
-      <c r="E283" s="159"/>
+      <c r="A283" s="159" t="s">
+        <v>288</v>
+      </c>
+      <c r="B283" s="160"/>
+      <c r="C283" s="160"/>
+      <c r="D283" s="160"/>
+      <c r="E283" s="161"/>
     </row>
     <row r="284" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A284" s="30" t="s">
@@ -6411,14 +6411,14 @@
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" s="32" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B292" s="5" t="s">
         <v>3</v>
       </c>
       <c r="C292" s="18"/>
       <c r="D292" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E292" s="21"/>
     </row>
@@ -6492,7 +6492,7 @@
     </row>
     <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B299" s="5" t="s">
         <v>118</v>
@@ -6574,7 +6574,7 @@
         <v>127</v>
       </c>
       <c r="B306" s="5" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="C306" s="24" t="s">
         <v>5</v>
@@ -6630,7 +6630,7 @@
       </c>
       <c r="C310" s="59"/>
       <c r="D310" s="59" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E310" s="47"/>
     </row>
@@ -6702,12 +6702,34 @@
       </c>
       <c r="C316" s="33"/>
       <c r="D316" s="11" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E316" s="34"/>
     </row>
   </sheetData>
   <mergeCells count="29">
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A14:E14"/>
+    <mergeCell ref="A21:E21"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="A3:E3"/>
+    <mergeCell ref="A53:E53"/>
+    <mergeCell ref="A61:E61"/>
+    <mergeCell ref="A89:E89"/>
+    <mergeCell ref="A94:E94"/>
+    <mergeCell ref="A125:E125"/>
+    <mergeCell ref="A140:E140"/>
+    <mergeCell ref="A157:E157"/>
+    <mergeCell ref="A167:E167"/>
+    <mergeCell ref="A173:E173"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A193:E193"/>
+    <mergeCell ref="A198:E198"/>
+    <mergeCell ref="A205:E205"/>
+    <mergeCell ref="A214:E214"/>
+    <mergeCell ref="A225:E225"/>
     <mergeCell ref="A303:E303"/>
     <mergeCell ref="A312:E312"/>
     <mergeCell ref="A234:E234"/>
@@ -6715,28 +6737,6 @@
     <mergeCell ref="A269:E269"/>
     <mergeCell ref="A277:E277"/>
     <mergeCell ref="A283:E283"/>
-    <mergeCell ref="A193:E193"/>
-    <mergeCell ref="A198:E198"/>
-    <mergeCell ref="A205:E205"/>
-    <mergeCell ref="A214:E214"/>
-    <mergeCell ref="A225:E225"/>
-    <mergeCell ref="A140:E140"/>
-    <mergeCell ref="A157:E157"/>
-    <mergeCell ref="A167:E167"/>
-    <mergeCell ref="A173:E173"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A53:E53"/>
-    <mergeCell ref="A61:E61"/>
-    <mergeCell ref="A89:E89"/>
-    <mergeCell ref="A94:E94"/>
-    <mergeCell ref="A125:E125"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A21:E21"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="A38:E38"/>
-    <mergeCell ref="A3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -6750,8 +6750,8 @@
   </sheetPr>
   <dimension ref="A1:H182"/>
   <sheetViews>
-    <sheetView topLeftCell="A156" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H45" sqref="A38:H45"/>
+    <sheetView tabSelected="1" topLeftCell="A156" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D170" sqref="D170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6790,19 +6790,19 @@
         <v>139</v>
       </c>
       <c r="D2" s="92" t="s">
+        <v>389</v>
+      </c>
+      <c r="E2" s="93" t="s">
+        <v>276</v>
+      </c>
+      <c r="F2" s="93" t="s">
+        <v>396</v>
+      </c>
+      <c r="G2" s="93" t="s">
+        <v>395</v>
+      </c>
+      <c r="H2" s="93" t="s">
         <v>390</v>
-      </c>
-      <c r="E2" s="93" t="s">
-        <v>277</v>
-      </c>
-      <c r="F2" s="93" t="s">
-        <v>397</v>
-      </c>
-      <c r="G2" s="93" t="s">
-        <v>396</v>
-      </c>
-      <c r="H2" s="93" t="s">
-        <v>391</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -6813,20 +6813,20 @@
         <v>140</v>
       </c>
       <c r="C3" s="106" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D3" s="107" t="s">
         <v>184</v>
       </c>
       <c r="E3" s="105" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F3" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G3" s="105"/>
       <c r="H3" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -6837,7 +6837,7 @@
         <v>141</v>
       </c>
       <c r="C4" s="111" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D4" s="112" t="s">
         <v>186</v>
@@ -6852,7 +6852,7 @@
         <v>5</v>
       </c>
       <c r="H4" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -6863,7 +6863,7 @@
         <v>142</v>
       </c>
       <c r="C5" s="111" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D5" s="112" t="s">
         <v>185</v>
@@ -6881,7 +6881,7 @@
         <v>140</v>
       </c>
       <c r="C6" s="111" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D6" s="112" t="s">
         <v>249</v>
@@ -6896,7 +6896,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -6907,7 +6907,7 @@
         <v>143</v>
       </c>
       <c r="C7" s="111" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D7" s="112" t="s">
         <v>187</v>
@@ -6922,7 +6922,7 @@
         <v>5</v>
       </c>
       <c r="H7" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -6933,7 +6933,7 @@
         <v>142</v>
       </c>
       <c r="C8" s="111" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D8" s="112" t="s">
         <v>188</v>
@@ -6946,7 +6946,7 @@
         <v>5</v>
       </c>
       <c r="H8" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -6957,13 +6957,13 @@
         <v>140</v>
       </c>
       <c r="C9" s="111" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D9" s="112" t="s">
         <v>190</v>
       </c>
       <c r="E9" s="110" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F9" s="110" t="s">
         <v>5</v>
@@ -6972,7 +6972,7 @@
         <v>5</v>
       </c>
       <c r="H9" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6983,13 +6983,13 @@
         <v>140</v>
       </c>
       <c r="C10" s="121" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D10" s="122" t="s">
         <v>189</v>
       </c>
       <c r="E10" s="120" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="F10" s="120" t="s">
         <v>5</v>
@@ -6998,7 +6998,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -7009,20 +7009,20 @@
         <v>140</v>
       </c>
       <c r="C11" s="96" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D11" s="127" t="s">
+        <v>403</v>
+      </c>
+      <c r="E11" s="95" t="s">
         <v>404</v>
-      </c>
-      <c r="E11" s="95" t="s">
-        <v>405</v>
       </c>
       <c r="F11" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G11" s="95"/>
       <c r="H11" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -7033,7 +7033,7 @@
         <v>141</v>
       </c>
       <c r="C12" s="52" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D12" s="53" t="s">
         <v>173</v>
@@ -7048,7 +7048,7 @@
         <v>5</v>
       </c>
       <c r="H12" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -7059,7 +7059,7 @@
         <v>142</v>
       </c>
       <c r="C13" s="52" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D13" s="53" t="s">
         <v>172</v>
@@ -7077,7 +7077,7 @@
         <v>140</v>
       </c>
       <c r="C14" s="52" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D14" s="53" t="s">
         <v>247</v>
@@ -7092,7 +7092,7 @@
         <v>5</v>
       </c>
       <c r="H14" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -7103,7 +7103,7 @@
         <v>143</v>
       </c>
       <c r="C15" s="52" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D15" s="53" t="s">
         <v>174</v>
@@ -7118,7 +7118,7 @@
         <v>5</v>
       </c>
       <c r="H15" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7129,7 +7129,7 @@
         <v>142</v>
       </c>
       <c r="C16" s="101" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D16" s="102" t="s">
         <v>175</v>
@@ -7142,7 +7142,7 @@
         <v>5</v>
       </c>
       <c r="H16" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -7153,20 +7153,20 @@
         <v>140</v>
       </c>
       <c r="C17" s="106" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D17" s="107" t="s">
         <v>223</v>
       </c>
       <c r="E17" s="105" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F17" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G17" s="105"/>
       <c r="H17" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -7177,7 +7177,7 @@
         <v>141</v>
       </c>
       <c r="C18" s="111" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D18" s="112" t="s">
         <v>225</v>
@@ -7192,7 +7192,7 @@
         <v>5</v>
       </c>
       <c r="H18" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -7203,7 +7203,7 @@
         <v>142</v>
       </c>
       <c r="C19" s="111" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="D19" s="112" t="s">
         <v>224</v>
@@ -7221,7 +7221,7 @@
         <v>140</v>
       </c>
       <c r="C20" s="111" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D20" s="112" t="s">
         <v>255</v>
@@ -7236,7 +7236,7 @@
         <v>5</v>
       </c>
       <c r="H20" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -7247,7 +7247,7 @@
         <v>143</v>
       </c>
       <c r="C21" s="111" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D21" s="112" t="s">
         <v>226</v>
@@ -7262,7 +7262,7 @@
         <v>5</v>
       </c>
       <c r="H21" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -7273,7 +7273,7 @@
         <v>142</v>
       </c>
       <c r="C22" s="111" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="D22" s="112" t="s">
         <v>227</v>
@@ -7286,7 +7286,7 @@
         <v>5</v>
       </c>
       <c r="H22" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -7297,13 +7297,13 @@
         <v>140</v>
       </c>
       <c r="C23" s="111" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="D23" s="112" t="s">
         <v>228</v>
       </c>
       <c r="E23" s="110" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F23" s="110" t="s">
         <v>5</v>
@@ -7312,7 +7312,7 @@
         <v>5</v>
       </c>
       <c r="H23" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7323,13 +7323,13 @@
         <v>140</v>
       </c>
       <c r="C24" s="121" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="D24" s="122" t="s">
         <v>228</v>
       </c>
       <c r="E24" s="120" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="F24" s="120" t="s">
         <v>5</v>
@@ -7338,48 +7338,48 @@
         <v>5</v>
       </c>
       <c r="H24" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="94" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B25" s="95" t="s">
         <v>140</v>
       </c>
       <c r="C25" s="96" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D25" s="127" t="s">
+        <v>524</v>
+      </c>
+      <c r="E25" s="95" t="s">
         <v>525</v>
-      </c>
-      <c r="E25" s="95" t="s">
-        <v>526</v>
       </c>
       <c r="F25" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G25" s="95"/>
       <c r="H25" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="55" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B26" s="50" t="s">
         <v>141</v>
       </c>
       <c r="C26" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D26" s="53" t="s">
         <v>159</v>
       </c>
       <c r="E26" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F26" s="50" t="s">
         <v>5</v>
@@ -7388,18 +7388,18 @@
         <v>5</v>
       </c>
       <c r="H26" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="55" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B27" s="50" t="s">
         <v>142</v>
       </c>
       <c r="C27" s="52" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="D27" s="53" t="s">
         <v>158</v>
@@ -7411,19 +7411,19 @@
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="55" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B28" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C28" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D28" s="53" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="E28" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F28" s="50" t="s">
         <v>5</v>
@@ -7432,24 +7432,24 @@
         <v>5</v>
       </c>
       <c r="H28" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="55" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B29" s="50" t="s">
         <v>143</v>
       </c>
       <c r="C29" s="52" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D29" s="53" t="s">
         <v>160</v>
       </c>
       <c r="E29" s="50" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F29" s="50" t="s">
         <v>5</v>
@@ -7458,18 +7458,18 @@
         <v>5</v>
       </c>
       <c r="H29" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="56" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="B30" s="57" t="s">
         <v>142</v>
       </c>
       <c r="C30" s="58" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
       <c r="D30" s="98" t="s">
         <v>161</v>
@@ -7482,7 +7482,7 @@
         <v>5</v>
       </c>
       <c r="H30" s="103" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -7493,20 +7493,20 @@
         <v>140</v>
       </c>
       <c r="C31" s="135" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D31" s="136" t="s">
+        <v>411</v>
+      </c>
+      <c r="E31" s="134" t="s">
         <v>412</v>
-      </c>
-      <c r="E31" s="134" t="s">
-        <v>413</v>
       </c>
       <c r="F31" s="134" t="s">
         <v>5</v>
       </c>
       <c r="G31" s="134"/>
       <c r="H31" s="146" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -7517,7 +7517,7 @@
         <v>141</v>
       </c>
       <c r="C32" s="111" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D32" s="112" t="s">
         <v>159</v>
@@ -7532,7 +7532,7 @@
         <v>5</v>
       </c>
       <c r="H32" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -7543,7 +7543,7 @@
         <v>142</v>
       </c>
       <c r="C33" s="111" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D33" s="112" t="s">
         <v>158</v>
@@ -7561,10 +7561,10 @@
         <v>140</v>
       </c>
       <c r="C34" s="111" t="s">
+        <v>414</v>
+      </c>
+      <c r="D34" s="112" t="s">
         <v>415</v>
-      </c>
-      <c r="D34" s="112" t="s">
-        <v>416</v>
       </c>
       <c r="E34" s="110" t="s">
         <v>89</v>
@@ -7576,7 +7576,7 @@
         <v>5</v>
       </c>
       <c r="H34" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -7587,7 +7587,7 @@
         <v>143</v>
       </c>
       <c r="C35" s="111" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D35" s="112" t="s">
         <v>160</v>
@@ -7602,7 +7602,7 @@
         <v>5</v>
       </c>
       <c r="H35" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
@@ -7613,7 +7613,7 @@
         <v>142</v>
       </c>
       <c r="C36" s="121" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="D36" s="122" t="s">
         <v>161</v>
@@ -7626,7 +7626,7 @@
         <v>5</v>
       </c>
       <c r="H36" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7637,13 +7637,13 @@
         <v>140</v>
       </c>
       <c r="C37" s="121" t="s">
+        <v>528</v>
+      </c>
+      <c r="D37" s="122" t="s">
         <v>529</v>
       </c>
-      <c r="D37" s="122" t="s">
-        <v>530</v>
-      </c>
       <c r="E37" s="120" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F37" s="120" t="s">
         <v>5</v>
@@ -7652,48 +7652,48 @@
         <v>5</v>
       </c>
       <c r="H37" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="137" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B38" s="138" t="s">
         <v>140</v>
       </c>
       <c r="C38" s="139" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D38" s="140" t="s">
+        <v>515</v>
+      </c>
+      <c r="E38" s="138" t="s">
         <v>516</v>
-      </c>
-      <c r="E38" s="138" t="s">
-        <v>517</v>
       </c>
       <c r="F38" s="138" t="s">
         <v>5</v>
       </c>
       <c r="G38" s="138"/>
       <c r="H38" s="141" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B39" s="142" t="s">
         <v>141</v>
       </c>
       <c r="C39" s="143" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D39" s="144" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="E39" s="142" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F39" s="142" t="s">
         <v>5</v>
@@ -7702,21 +7702,21 @@
         <v>5</v>
       </c>
       <c r="H39" s="145" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B40" s="142" t="s">
         <v>142</v>
       </c>
       <c r="C40" s="143" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="D40" s="144" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="E40" s="142"/>
       <c r="F40" s="142"/>
@@ -7725,16 +7725,16 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B41" s="142" t="s">
         <v>142</v>
       </c>
       <c r="C41" s="143" t="s">
+        <v>532</v>
+      </c>
+      <c r="D41" s="144" t="s">
         <v>533</v>
-      </c>
-      <c r="D41" s="144" t="s">
-        <v>534</v>
       </c>
       <c r="E41" s="142"/>
       <c r="F41" s="142" t="s">
@@ -7742,24 +7742,24 @@
       </c>
       <c r="G41" s="142"/>
       <c r="H41" s="145" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B42" s="142" t="s">
         <v>141</v>
       </c>
       <c r="C42" s="143" t="s">
+        <v>530</v>
+      </c>
+      <c r="D42" s="144" t="s">
         <v>531</v>
       </c>
-      <c r="D42" s="144" t="s">
-        <v>532</v>
-      </c>
       <c r="E42" s="142" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="F42" s="142" t="s">
         <v>5</v>
@@ -7768,24 +7768,24 @@
         <v>5</v>
       </c>
       <c r="H42" s="145" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B43" s="142" t="s">
         <v>140</v>
       </c>
       <c r="C43" s="143" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="D43" s="144" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
       <c r="E43" s="142" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F43" s="142" t="s">
         <v>5</v>
@@ -7794,24 +7794,24 @@
         <v>5</v>
       </c>
       <c r="H43" s="145" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" s="147" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B44" s="142" t="s">
         <v>140</v>
       </c>
       <c r="C44" s="143" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="D44" s="144" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="E44" s="142" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="F44" s="142" t="s">
         <v>5</v>
@@ -7820,24 +7820,24 @@
         <v>5</v>
       </c>
       <c r="H44" s="145" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="148" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="B45" s="149" t="s">
         <v>140</v>
       </c>
       <c r="C45" s="150" t="s">
+        <v>534</v>
+      </c>
+      <c r="D45" s="151" t="s">
         <v>535</v>
       </c>
-      <c r="D45" s="151" t="s">
-        <v>536</v>
-      </c>
       <c r="E45" s="149" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F45" s="149" t="s">
         <v>5</v>
@@ -7846,7 +7846,7 @@
         <v>5</v>
       </c>
       <c r="H45" s="152" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
@@ -7857,20 +7857,20 @@
         <v>140</v>
       </c>
       <c r="C46" s="135" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D46" s="136" t="s">
         <v>214</v>
       </c>
       <c r="E46" s="134" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F46" s="134" t="s">
         <v>5</v>
       </c>
       <c r="G46" s="134"/>
       <c r="H46" s="146" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
@@ -7881,7 +7881,7 @@
         <v>141</v>
       </c>
       <c r="C47" s="111" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D47" s="112" t="s">
         <v>216</v>
@@ -7896,7 +7896,7 @@
         <v>5</v>
       </c>
       <c r="H47" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -7907,7 +7907,7 @@
         <v>142</v>
       </c>
       <c r="C48" s="111" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="D48" s="112" t="s">
         <v>215</v>
@@ -7925,7 +7925,7 @@
         <v>140</v>
       </c>
       <c r="C49" s="111" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D49" s="112" t="s">
         <v>254</v>
@@ -7940,7 +7940,7 @@
         <v>5</v>
       </c>
       <c r="H49" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
@@ -7951,7 +7951,7 @@
         <v>143</v>
       </c>
       <c r="C50" s="111" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D50" s="112" t="s">
         <v>217</v>
@@ -7966,7 +7966,7 @@
         <v>5</v>
       </c>
       <c r="H50" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
@@ -7977,7 +7977,7 @@
         <v>142</v>
       </c>
       <c r="C51" s="111" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="D51" s="112" t="s">
         <v>218</v>
@@ -7990,7 +7990,7 @@
         <v>5</v>
       </c>
       <c r="H51" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
@@ -8001,13 +8001,13 @@
         <v>140</v>
       </c>
       <c r="C52" s="111" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="D52" s="112" t="s">
         <v>220</v>
       </c>
       <c r="E52" s="110" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F52" s="110" t="s">
         <v>5</v>
@@ -8016,7 +8016,7 @@
         <v>5</v>
       </c>
       <c r="H52" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
@@ -8027,13 +8027,13 @@
         <v>140</v>
       </c>
       <c r="C53" s="111" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="D53" s="112" t="s">
         <v>222</v>
       </c>
       <c r="E53" s="110" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F53" s="110" t="s">
         <v>5</v>
@@ -8042,7 +8042,7 @@
         <v>5</v>
       </c>
       <c r="H53" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
@@ -8053,13 +8053,13 @@
         <v>140</v>
       </c>
       <c r="C54" s="111" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="D54" s="112" t="s">
         <v>219</v>
       </c>
       <c r="E54" s="110" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F54" s="110" t="s">
         <v>5</v>
@@ -8068,7 +8068,7 @@
         <v>5</v>
       </c>
       <c r="H54" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8079,13 +8079,13 @@
         <v>140</v>
       </c>
       <c r="C55" s="121" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D55" s="122" t="s">
         <v>221</v>
       </c>
       <c r="E55" s="120" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="F55" s="120" t="s">
         <v>5</v>
@@ -8094,7 +8094,7 @@
         <v>5</v>
       </c>
       <c r="H55" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.25">
@@ -8108,17 +8108,17 @@
         <v>208</v>
       </c>
       <c r="D56" s="97" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="E56" s="95" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="F56" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G56" s="95"/>
       <c r="H56" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.25">
@@ -8144,7 +8144,7 @@
         <v>5</v>
       </c>
       <c r="H57" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.25">
@@ -8188,7 +8188,7 @@
         <v>5</v>
       </c>
       <c r="H59" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.25">
@@ -8214,7 +8214,7 @@
         <v>5</v>
       </c>
       <c r="H60" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8238,7 +8238,7 @@
         <v>5</v>
       </c>
       <c r="H61" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.25">
@@ -8249,20 +8249,20 @@
         <v>140</v>
       </c>
       <c r="C62" s="106" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D62" s="107" t="s">
+        <v>429</v>
+      </c>
+      <c r="E62" s="105" t="s">
         <v>430</v>
-      </c>
-      <c r="E62" s="105" t="s">
-        <v>431</v>
       </c>
       <c r="F62" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G62" s="105"/>
       <c r="H62" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.25">
@@ -8273,7 +8273,7 @@
         <v>141</v>
       </c>
       <c r="C63" s="111" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D63" s="112" t="s">
         <v>191</v>
@@ -8288,7 +8288,7 @@
         <v>5</v>
       </c>
       <c r="H63" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.25">
@@ -8299,7 +8299,7 @@
         <v>142</v>
       </c>
       <c r="C64" s="111" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D64" s="112" t="s">
         <v>197</v>
@@ -8317,10 +8317,10 @@
         <v>140</v>
       </c>
       <c r="C65" s="111" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D65" s="112" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="E65" s="110" t="s">
         <v>38</v>
@@ -8332,7 +8332,7 @@
         <v>5</v>
       </c>
       <c r="H65" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.25">
@@ -8343,7 +8343,7 @@
         <v>143</v>
       </c>
       <c r="C66" s="111" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D66" s="112" t="s">
         <v>192</v>
@@ -8358,7 +8358,7 @@
         <v>5</v>
       </c>
       <c r="H66" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.25">
@@ -8369,7 +8369,7 @@
         <v>142</v>
       </c>
       <c r="C67" s="111" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="D67" s="112" t="s">
         <v>193</v>
@@ -8382,7 +8382,7 @@
         <v>5</v>
       </c>
       <c r="H67" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.25">
@@ -8393,10 +8393,10 @@
         <v>143</v>
       </c>
       <c r="C68" s="111" t="s">
+        <v>431</v>
+      </c>
+      <c r="D68" s="112" t="s">
         <v>432</v>
-      </c>
-      <c r="D68" s="112" t="s">
-        <v>433</v>
       </c>
       <c r="E68" s="110" t="s">
         <v>38</v>
@@ -8408,7 +8408,7 @@
         <v>5</v>
       </c>
       <c r="H68" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.25">
@@ -8419,10 +8419,10 @@
         <v>143</v>
       </c>
       <c r="C69" s="111" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="D69" s="112" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E69" s="110" t="s">
         <v>38</v>
@@ -8434,7 +8434,7 @@
         <v>5</v>
       </c>
       <c r="H69" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.25">
@@ -8445,10 +8445,10 @@
         <v>143</v>
       </c>
       <c r="C70" s="111" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="D70" s="112" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="E70" s="110" t="s">
         <v>38</v>
@@ -8460,7 +8460,7 @@
         <v>5</v>
       </c>
       <c r="H70" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8471,10 +8471,10 @@
         <v>143</v>
       </c>
       <c r="C71" s="121" t="s">
+        <v>434</v>
+      </c>
+      <c r="D71" s="122" t="s">
         <v>435</v>
-      </c>
-      <c r="D71" s="122" t="s">
-        <v>436</v>
       </c>
       <c r="E71" s="120" t="s">
         <v>38</v>
@@ -8486,7 +8486,7 @@
         <v>5</v>
       </c>
       <c r="H71" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -8497,20 +8497,20 @@
         <v>140</v>
       </c>
       <c r="C72" s="96" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D72" s="97" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="E72" s="95" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="F72" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G72" s="95"/>
       <c r="H72" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
@@ -8521,7 +8521,7 @@
         <v>141</v>
       </c>
       <c r="C73" s="52" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D73" s="51" t="s">
         <v>194</v>
@@ -8536,7 +8536,7 @@
         <v>5</v>
       </c>
       <c r="H73" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.25">
@@ -8547,7 +8547,7 @@
         <v>142</v>
       </c>
       <c r="C74" s="52" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D74" s="51" t="s">
         <v>198</v>
@@ -8565,7 +8565,7 @@
         <v>140</v>
       </c>
       <c r="C75" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D75" s="51" t="s">
         <v>250</v>
@@ -8580,7 +8580,7 @@
         <v>5</v>
       </c>
       <c r="H75" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
@@ -8591,7 +8591,7 @@
         <v>143</v>
       </c>
       <c r="C76" s="52" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D76" s="51" t="s">
         <v>195</v>
@@ -8606,7 +8606,7 @@
         <v>5</v>
       </c>
       <c r="H76" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8617,7 +8617,7 @@
         <v>142</v>
       </c>
       <c r="C77" s="101" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D77" s="125" t="s">
         <v>196</v>
@@ -8630,7 +8630,7 @@
         <v>5</v>
       </c>
       <c r="H77" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
@@ -8641,20 +8641,20 @@
         <v>140</v>
       </c>
       <c r="C78" s="106" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D78" s="107" t="s">
+        <v>438</v>
+      </c>
+      <c r="E78" s="105" t="s">
         <v>439</v>
-      </c>
-      <c r="E78" s="105" t="s">
-        <v>440</v>
       </c>
       <c r="F78" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G78" s="105"/>
       <c r="H78" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
@@ -8665,7 +8665,7 @@
         <v>141</v>
       </c>
       <c r="C79" s="111" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D79" s="112" t="s">
         <v>200</v>
@@ -8680,7 +8680,7 @@
         <v>5</v>
       </c>
       <c r="H79" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.25">
@@ -8691,7 +8691,7 @@
         <v>142</v>
       </c>
       <c r="C80" s="111" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D80" s="112" t="s">
         <v>199</v>
@@ -8709,7 +8709,7 @@
         <v>140</v>
       </c>
       <c r="C81" s="111" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D81" s="112" t="s">
         <v>251</v>
@@ -8724,7 +8724,7 @@
         <v>5</v>
       </c>
       <c r="H81" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
@@ -8735,7 +8735,7 @@
         <v>143</v>
       </c>
       <c r="C82" s="111" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D82" s="112" t="s">
         <v>201</v>
@@ -8750,7 +8750,7 @@
         <v>5</v>
       </c>
       <c r="H82" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8761,7 +8761,7 @@
         <v>142</v>
       </c>
       <c r="C83" s="116" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D83" s="117" t="s">
         <v>202</v>
@@ -8774,48 +8774,48 @@
         <v>5</v>
       </c>
       <c r="H83" s="118" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="84" spans="1:8" s="128" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="94" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B84" s="95" t="s">
         <v>140</v>
       </c>
       <c r="C84" s="96" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D84" s="127" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="E84" s="95" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F84" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G84" s="95"/>
       <c r="H84" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="85" spans="1:8" s="128" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A85" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B85" s="50" t="s">
         <v>141</v>
       </c>
       <c r="C85" s="52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D85" s="53" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="E85" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F85" s="50" t="s">
         <v>5</v>
@@ -8824,21 +8824,21 @@
         <v>5</v>
       </c>
       <c r="H85" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="86" spans="1:8" s="128" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A86" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B86" s="50" t="s">
         <v>142</v>
       </c>
       <c r="C86" s="52" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="D86" s="53" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="E86" s="50"/>
       <c r="F86" s="50"/>
@@ -8847,19 +8847,19 @@
     </row>
     <row r="87" spans="1:8" s="128" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B87" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C87" s="52" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D87" s="53" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="E87" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F87" s="50" t="s">
         <v>5</v>
@@ -8868,24 +8868,24 @@
         <v>5</v>
       </c>
       <c r="H87" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="88" spans="1:8" s="128" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A88" s="55" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B88" s="50" t="s">
         <v>143</v>
       </c>
       <c r="C88" s="52" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D88" s="53" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="E88" s="50" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="F88" s="50" t="s">
         <v>5</v>
@@ -8894,21 +8894,21 @@
         <v>5</v>
       </c>
       <c r="H88" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="89" spans="1:8" s="128" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="124" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B89" s="100" t="s">
         <v>142</v>
       </c>
       <c r="C89" s="101" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="D89" s="102" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="E89" s="100"/>
       <c r="F89" s="100" t="s">
@@ -8918,7 +8918,7 @@
         <v>5</v>
       </c>
       <c r="H89" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
@@ -8929,20 +8929,20 @@
         <v>140</v>
       </c>
       <c r="C90" s="106" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D90" s="107" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="E90" s="105" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="F90" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G90" s="105"/>
       <c r="H90" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
@@ -8953,7 +8953,7 @@
         <v>141</v>
       </c>
       <c r="C91" s="111" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D91" s="112" t="s">
         <v>163</v>
@@ -8968,7 +8968,7 @@
         <v>5</v>
       </c>
       <c r="H91" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
@@ -8979,7 +8979,7 @@
         <v>142</v>
       </c>
       <c r="C92" s="111" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="D92" s="112" t="s">
         <v>162</v>
@@ -8997,7 +8997,7 @@
         <v>140</v>
       </c>
       <c r="C93" s="111" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D93" s="112" t="s">
         <v>245</v>
@@ -9012,7 +9012,7 @@
         <v>5</v>
       </c>
       <c r="H93" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.25">
@@ -9023,7 +9023,7 @@
         <v>143</v>
       </c>
       <c r="C94" s="111" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D94" s="112" t="s">
         <v>164</v>
@@ -9038,7 +9038,7 @@
         <v>5</v>
       </c>
       <c r="H94" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9049,7 +9049,7 @@
         <v>142</v>
       </c>
       <c r="C95" s="121" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="D95" s="122" t="s">
         <v>165</v>
@@ -9062,7 +9062,7 @@
         <v>5</v>
       </c>
       <c r="H95" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.25">
@@ -9073,20 +9073,20 @@
         <v>140</v>
       </c>
       <c r="C96" s="96" t="s">
+        <v>456</v>
+      </c>
+      <c r="D96" s="97" t="s">
         <v>457</v>
       </c>
-      <c r="D96" s="97" t="s">
+      <c r="E96" s="95" t="s">
         <v>458</v>
-      </c>
-      <c r="E96" s="95" t="s">
-        <v>459</v>
       </c>
       <c r="F96" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G96" s="95"/>
       <c r="H96" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.25">
@@ -9097,7 +9097,7 @@
         <v>141</v>
       </c>
       <c r="C97" s="52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D97" s="51" t="s">
         <v>167</v>
@@ -9112,7 +9112,7 @@
         <v>5</v>
       </c>
       <c r="H97" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.25">
@@ -9123,10 +9123,10 @@
         <v>142</v>
       </c>
       <c r="C98" s="52" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="D98" s="51" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="E98" s="50"/>
       <c r="F98" s="50"/>
@@ -9141,10 +9141,10 @@
         <v>142</v>
       </c>
       <c r="C99" s="52" t="s">
+        <v>459</v>
+      </c>
+      <c r="D99" s="51" t="s">
         <v>460</v>
-      </c>
-      <c r="D99" s="51" t="s">
-        <v>461</v>
       </c>
       <c r="E99" s="50"/>
       <c r="F99" s="50" t="s">
@@ -9154,7 +9154,7 @@
         <v>5</v>
       </c>
       <c r="H99" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
@@ -9165,14 +9165,14 @@
         <v>140</v>
       </c>
       <c r="C100" s="52" t="s">
+        <v>461</v>
+      </c>
+      <c r="D100" s="51" t="s">
+        <v>463</v>
+      </c>
+      <c r="E100" s="50" t="s">
         <v>462</v>
       </c>
-      <c r="D100" s="51" t="s">
-        <v>464</v>
-      </c>
-      <c r="E100" s="50" t="s">
-        <v>463</v>
-      </c>
       <c r="F100" s="50" t="s">
         <v>5</v>
       </c>
@@ -9180,7 +9180,7 @@
         <v>5</v>
       </c>
       <c r="H100" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9191,14 +9191,14 @@
         <v>140</v>
       </c>
       <c r="C101" s="101" t="s">
+        <v>464</v>
+      </c>
+      <c r="D101" s="125" t="s">
         <v>465</v>
       </c>
-      <c r="D101" s="125" t="s">
+      <c r="E101" s="100" t="s">
         <v>466</v>
       </c>
-      <c r="E101" s="100" t="s">
-        <v>467</v>
-      </c>
       <c r="F101" s="100" t="s">
         <v>5</v>
       </c>
@@ -9206,7 +9206,7 @@
         <v>5</v>
       </c>
       <c r="H101" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
@@ -9217,20 +9217,20 @@
         <v>140</v>
       </c>
       <c r="C102" s="106" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D102" s="107" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E102" s="105" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="F102" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G102" s="105"/>
       <c r="H102" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
@@ -9241,7 +9241,7 @@
         <v>141</v>
       </c>
       <c r="C103" s="111" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D103" s="112" t="s">
         <v>169</v>
@@ -9256,7 +9256,7 @@
         <v>5</v>
       </c>
       <c r="H103" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
@@ -9267,7 +9267,7 @@
         <v>142</v>
       </c>
       <c r="C104" s="111" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="D104" s="112" t="s">
         <v>168</v>
@@ -9285,7 +9285,7 @@
         <v>140</v>
       </c>
       <c r="C105" s="111" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D105" s="112" t="s">
         <v>246</v>
@@ -9300,7 +9300,7 @@
         <v>5</v>
       </c>
       <c r="H105" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
@@ -9311,7 +9311,7 @@
         <v>143</v>
       </c>
       <c r="C106" s="111" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D106" s="112" t="s">
         <v>170</v>
@@ -9326,7 +9326,7 @@
         <v>5</v>
       </c>
       <c r="H106" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9337,7 +9337,7 @@
         <v>142</v>
       </c>
       <c r="C107" s="121" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="D107" s="122" t="s">
         <v>171</v>
@@ -9350,7 +9350,7 @@
         <v>5</v>
       </c>
       <c r="H107" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
@@ -9367,14 +9367,14 @@
         <v>236</v>
       </c>
       <c r="E108" s="95" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F108" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G108" s="95"/>
       <c r="H108" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
@@ -9400,7 +9400,7 @@
         <v>5</v>
       </c>
       <c r="H109" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
@@ -9444,7 +9444,7 @@
         <v>5</v>
       </c>
       <c r="H111" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
@@ -9470,7 +9470,7 @@
         <v>5</v>
       </c>
       <c r="H112" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.25">
@@ -9494,7 +9494,7 @@
         <v>5</v>
       </c>
       <c r="H113" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.25">
@@ -9505,13 +9505,13 @@
         <v>140</v>
       </c>
       <c r="C114" s="52" t="s">
+        <v>274</v>
+      </c>
+      <c r="D114" s="51" t="s">
         <v>275</v>
       </c>
-      <c r="D114" s="51" t="s">
-        <v>276</v>
-      </c>
       <c r="E114" s="50" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F114" s="50" t="s">
         <v>5</v>
@@ -9520,7 +9520,7 @@
         <v>5</v>
       </c>
       <c r="H114" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="115" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9537,7 +9537,7 @@
         <v>243</v>
       </c>
       <c r="E115" s="100" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="F115" s="100" t="s">
         <v>5</v>
@@ -9546,7 +9546,7 @@
         <v>5</v>
       </c>
       <c r="H115" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.25">
@@ -9557,20 +9557,20 @@
         <v>140</v>
       </c>
       <c r="C116" s="106" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D116" s="107" t="s">
         <v>229</v>
       </c>
       <c r="E116" s="105" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F116" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G116" s="105"/>
       <c r="H116" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.25">
@@ -9581,7 +9581,7 @@
         <v>141</v>
       </c>
       <c r="C117" s="111" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D117" s="112" t="s">
         <v>231</v>
@@ -9596,7 +9596,7 @@
         <v>5</v>
       </c>
       <c r="H117" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.25">
@@ -9607,7 +9607,7 @@
         <v>142</v>
       </c>
       <c r="C118" s="111" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="D118" s="112" t="s">
         <v>230</v>
@@ -9625,7 +9625,7 @@
         <v>140</v>
       </c>
       <c r="C119" s="111" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D119" s="112" t="s">
         <v>256</v>
@@ -9640,7 +9640,7 @@
         <v>5</v>
       </c>
       <c r="H119" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.25">
@@ -9651,7 +9651,7 @@
         <v>143</v>
       </c>
       <c r="C120" s="111" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D120" s="112" t="s">
         <v>232</v>
@@ -9666,7 +9666,7 @@
         <v>5</v>
       </c>
       <c r="H120" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.25">
@@ -9677,7 +9677,7 @@
         <v>142</v>
       </c>
       <c r="C121" s="111" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="D121" s="112" t="s">
         <v>233</v>
@@ -9690,7 +9690,7 @@
         <v>5</v>
       </c>
       <c r="H121" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="122" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9701,13 +9701,13 @@
         <v>140</v>
       </c>
       <c r="C122" s="121" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="D122" s="122" t="s">
         <v>234</v>
       </c>
       <c r="E122" s="120" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F122" s="120" t="s">
         <v>5</v>
@@ -9716,7 +9716,7 @@
         <v>5</v>
       </c>
       <c r="H122" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.25">
@@ -9727,20 +9727,20 @@
         <v>140</v>
       </c>
       <c r="C123" s="96" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D123" s="97" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="E123" s="95" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F123" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G123" s="95"/>
       <c r="H123" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.25">
@@ -9751,7 +9751,7 @@
         <v>141</v>
       </c>
       <c r="C124" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D124" s="51" t="s">
         <v>204</v>
@@ -9766,7 +9766,7 @@
         <v>5</v>
       </c>
       <c r="H124" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.25">
@@ -9777,7 +9777,7 @@
         <v>142</v>
       </c>
       <c r="C125" s="52" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="D125" s="51" t="s">
         <v>203</v>
@@ -9795,7 +9795,7 @@
         <v>140</v>
       </c>
       <c r="C126" s="52" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D126" s="51" t="s">
         <v>252</v>
@@ -9810,7 +9810,7 @@
         <v>5</v>
       </c>
       <c r="H126" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.25">
@@ -9821,7 +9821,7 @@
         <v>143</v>
       </c>
       <c r="C127" s="52" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D127" s="51" t="s">
         <v>205</v>
@@ -9836,7 +9836,7 @@
         <v>5</v>
       </c>
       <c r="H127" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.25">
@@ -9847,7 +9847,7 @@
         <v>142</v>
       </c>
       <c r="C128" s="52" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="D128" s="51" t="s">
         <v>206</v>
@@ -9860,7 +9860,7 @@
         <v>5</v>
       </c>
       <c r="H128" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.25">
@@ -9871,13 +9871,13 @@
         <v>140</v>
       </c>
       <c r="C129" s="52" t="s">
+        <v>480</v>
+      </c>
+      <c r="D129" s="51" t="s">
         <v>481</v>
       </c>
-      <c r="D129" s="51" t="s">
-        <v>482</v>
-      </c>
       <c r="E129" s="50" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="F129" s="50" t="s">
         <v>5</v>
@@ -9886,7 +9886,7 @@
         <v>5</v>
       </c>
       <c r="H129" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="130" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9897,10 +9897,10 @@
         <v>143</v>
       </c>
       <c r="C130" s="101" t="s">
+        <v>482</v>
+      </c>
+      <c r="D130" s="125" t="s">
         <v>483</v>
-      </c>
-      <c r="D130" s="125" t="s">
-        <v>484</v>
       </c>
       <c r="E130" s="100" t="s">
         <v>103</v>
@@ -9912,7 +9912,7 @@
         <v>5</v>
       </c>
       <c r="H130" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.25">
@@ -9923,20 +9923,20 @@
         <v>140</v>
       </c>
       <c r="C131" s="106" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D131" s="107" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="E131" s="105" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="F131" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G131" s="105"/>
       <c r="H131" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.25">
@@ -9947,7 +9947,7 @@
         <v>141</v>
       </c>
       <c r="C132" s="111" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D132" s="112" t="s">
         <v>149</v>
@@ -9962,7 +9962,7 @@
         <v>5</v>
       </c>
       <c r="H132" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.25">
@@ -9973,7 +9973,7 @@
         <v>142</v>
       </c>
       <c r="C133" s="111" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="D133" s="112" t="s">
         <v>148</v>
@@ -9991,10 +9991,10 @@
         <v>140</v>
       </c>
       <c r="C134" s="111" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D134" s="112" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="E134" s="110" t="s">
         <v>81</v>
@@ -10006,7 +10006,7 @@
         <v>5</v>
       </c>
       <c r="H134" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.25">
@@ -10017,7 +10017,7 @@
         <v>143</v>
       </c>
       <c r="C135" s="111" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D135" s="112" t="s">
         <v>150</v>
@@ -10032,7 +10032,7 @@
         <v>5</v>
       </c>
       <c r="H135" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="136" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10043,7 +10043,7 @@
         <v>142</v>
       </c>
       <c r="C136" s="121" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="D136" s="122" t="s">
         <v>151</v>
@@ -10056,7 +10056,7 @@
         <v>5</v>
       </c>
       <c r="H136" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.25">
@@ -10073,14 +10073,14 @@
         <v>179</v>
       </c>
       <c r="E137" s="95" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="F137" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G137" s="95"/>
       <c r="H137" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.25">
@@ -10106,7 +10106,7 @@
         <v>5</v>
       </c>
       <c r="H138" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.25">
@@ -10150,7 +10150,7 @@
         <v>5</v>
       </c>
       <c r="H140" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.25">
@@ -10176,7 +10176,7 @@
         <v>5</v>
       </c>
       <c r="H141" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="142" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10200,7 +10200,7 @@
         <v>5</v>
       </c>
       <c r="H142" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.25">
@@ -10214,7 +10214,7 @@
         <v>152</v>
       </c>
       <c r="D143" s="107" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="E143" s="105" t="s">
         <v>88</v>
@@ -10224,7 +10224,7 @@
       </c>
       <c r="G143" s="105"/>
       <c r="H143" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.25">
@@ -10250,7 +10250,7 @@
         <v>5</v>
       </c>
       <c r="H144" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -10294,7 +10294,7 @@
         <v>5</v>
       </c>
       <c r="H146" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -10320,7 +10320,7 @@
         <v>5</v>
       </c>
       <c r="H147" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="148" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10344,48 +10344,48 @@
         <v>5</v>
       </c>
       <c r="H148" s="123" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="149" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A149" s="129" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B149" s="130" t="s">
         <v>140</v>
       </c>
       <c r="C149" s="131" t="s">
+        <v>293</v>
+      </c>
+      <c r="D149" s="132" t="s">
         <v>294</v>
       </c>
-      <c r="D149" s="132" t="s">
-        <v>295</v>
-      </c>
       <c r="E149" s="130" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="F149" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G149" s="95"/>
       <c r="H149" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="150" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A150" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B150" s="62" t="s">
         <v>141</v>
       </c>
       <c r="C150" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D150" s="64" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="E150" s="62" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F150" s="50" t="s">
         <v>5</v>
@@ -10394,21 +10394,21 @@
         <v>5</v>
       </c>
       <c r="H150" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="151" spans="1:8" s="65" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A151" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B151" s="62" t="s">
         <v>142</v>
       </c>
       <c r="C151" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="D151" s="64" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="E151" s="62"/>
       <c r="F151" s="50"/>
@@ -10417,19 +10417,19 @@
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B152" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C152" s="63" t="s">
+        <v>306</v>
+      </c>
+      <c r="D152" s="53" t="s">
         <v>307</v>
       </c>
-      <c r="D152" s="53" t="s">
-        <v>308</v>
-      </c>
       <c r="E152" s="50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F152" s="50" t="s">
         <v>5</v>
@@ -10438,24 +10438,24 @@
         <v>5</v>
       </c>
       <c r="H152" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B153" s="50" t="s">
         <v>143</v>
       </c>
       <c r="C153" s="63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D153" s="53" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="E153" s="50" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="F153" s="50" t="s">
         <v>5</v>
@@ -10464,21 +10464,21 @@
         <v>5</v>
       </c>
       <c r="H153" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" s="61" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B154" s="50" t="s">
         <v>142</v>
       </c>
       <c r="C154" s="63" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D154" s="53" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="E154" s="50"/>
       <c r="F154" s="50" t="s">
@@ -10488,21 +10488,21 @@
         <v>5</v>
       </c>
       <c r="H154" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B155" s="50" t="s">
         <v>142</v>
       </c>
       <c r="C155" s="52" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="D155" s="53" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="E155" s="50"/>
       <c r="F155" s="50"/>
@@ -10511,19 +10511,19 @@
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B156" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C156" s="52" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D156" s="53" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="E156" s="50" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="F156" s="50" t="s">
         <v>5</v>
@@ -10532,24 +10532,24 @@
         <v>5</v>
       </c>
       <c r="H156" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B157" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C157" s="52" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="D157" s="53" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="E157" s="50" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F157" s="50" t="s">
         <v>5</v>
@@ -10558,24 +10558,24 @@
         <v>5</v>
       </c>
       <c r="H157" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" s="55" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B158" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C158" s="52" t="s">
+        <v>301</v>
+      </c>
+      <c r="D158" s="53" t="s">
+        <v>271</v>
+      </c>
+      <c r="E158" s="50" t="s">
         <v>302</v>
-      </c>
-      <c r="D158" s="53" t="s">
-        <v>272</v>
-      </c>
-      <c r="E158" s="50" t="s">
-        <v>303</v>
       </c>
       <c r="F158" s="50"/>
       <c r="G158" s="50"/>
@@ -10583,16 +10583,16 @@
     </row>
     <row r="159" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A159" s="124" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B159" s="100" t="s">
         <v>142</v>
       </c>
       <c r="C159" s="101" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D159" s="102" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E159" s="100"/>
       <c r="F159" s="100"/>
@@ -10607,20 +10607,20 @@
         <v>140</v>
       </c>
       <c r="C160" s="106" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D160" s="107" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="E160" s="105" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F160" s="105" t="s">
         <v>5</v>
       </c>
       <c r="G160" s="105"/>
       <c r="H160" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.25">
@@ -10631,10 +10631,10 @@
         <v>142</v>
       </c>
       <c r="C161" s="111" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="D161" s="112" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="E161" s="110"/>
       <c r="F161" s="110"/>
@@ -10649,7 +10649,7 @@
         <v>140</v>
       </c>
       <c r="C162" s="111" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D162" s="112" t="s">
         <v>144</v>
@@ -10664,7 +10664,7 @@
         <v>5</v>
       </c>
       <c r="H162" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.25">
@@ -10675,7 +10675,7 @@
         <v>143</v>
       </c>
       <c r="C163" s="111" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D163" s="112" t="s">
         <v>145</v>
@@ -10690,7 +10690,7 @@
         <v>5</v>
       </c>
       <c r="H163" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.25">
@@ -10701,7 +10701,7 @@
         <v>142</v>
       </c>
       <c r="C164" s="111" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="D164" s="112" t="s">
         <v>146</v>
@@ -10714,7 +10714,7 @@
         <v>5</v>
       </c>
       <c r="H164" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.25">
@@ -10725,13 +10725,13 @@
         <v>140</v>
       </c>
       <c r="C165" s="111" t="s">
+        <v>497</v>
+      </c>
+      <c r="D165" s="112" t="s">
         <v>498</v>
       </c>
-      <c r="D165" s="112" t="s">
-        <v>499</v>
-      </c>
       <c r="E165" s="110" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="F165" s="110" t="s">
         <v>5</v>
@@ -10740,7 +10740,7 @@
         <v>5</v>
       </c>
       <c r="H165" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.25">
@@ -10751,10 +10751,10 @@
         <v>141</v>
       </c>
       <c r="C166" s="111" t="s">
+        <v>499</v>
+      </c>
+      <c r="D166" s="112" t="s">
         <v>500</v>
-      </c>
-      <c r="D166" s="112" t="s">
-        <v>501</v>
       </c>
       <c r="E166" s="110" t="s">
         <v>0</v>
@@ -10766,7 +10766,7 @@
         <v>5</v>
       </c>
       <c r="H166" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.25">
@@ -10777,14 +10777,14 @@
         <v>141</v>
       </c>
       <c r="C167" s="111" t="s">
+        <v>501</v>
+      </c>
+      <c r="D167" s="112" t="s">
         <v>502</v>
       </c>
-      <c r="D167" s="112" t="s">
+      <c r="E167" s="110" t="s">
         <v>503</v>
       </c>
-      <c r="E167" s="110" t="s">
-        <v>504</v>
-      </c>
       <c r="F167" s="110" t="s">
         <v>5</v>
       </c>
@@ -10792,7 +10792,7 @@
         <v>5</v>
       </c>
       <c r="H167" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="168" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10803,10 +10803,10 @@
         <v>141</v>
       </c>
       <c r="C168" s="111" t="s">
+        <v>504</v>
+      </c>
+      <c r="D168" s="112" t="s">
         <v>505</v>
-      </c>
-      <c r="D168" s="112" t="s">
-        <v>506</v>
       </c>
       <c r="E168" s="110"/>
       <c r="F168" s="110"/>
@@ -10821,20 +10821,20 @@
         <v>140</v>
       </c>
       <c r="C169" s="96" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D169" s="97" t="s">
         <v>268</v>
       </c>
       <c r="E169" s="95" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F169" s="95" t="s">
         <v>5</v>
       </c>
       <c r="G169" s="95"/>
       <c r="H169" s="99" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.25">
@@ -10845,10 +10845,10 @@
         <v>141</v>
       </c>
       <c r="C170" s="52" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D170" s="51" t="s">
-        <v>270</v>
+        <v>536</v>
       </c>
       <c r="E170" s="50" t="s">
         <v>264</v>
@@ -10860,7 +10860,7 @@
         <v>5</v>
       </c>
       <c r="H170" s="60" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.25">
@@ -10871,7 +10871,7 @@
         <v>142</v>
       </c>
       <c r="C171" s="52" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="D171" s="51" t="s">
         <v>269</v>
@@ -10889,7 +10889,7 @@
         <v>140</v>
       </c>
       <c r="C172" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D172" s="51" t="s">
         <v>265</v>
@@ -10904,7 +10904,7 @@
         <v>5</v>
       </c>
       <c r="H172" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.25">
@@ -10915,7 +10915,7 @@
         <v>143</v>
       </c>
       <c r="C173" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D173" s="51" t="s">
         <v>266</v>
@@ -10930,7 +10930,7 @@
         <v>5</v>
       </c>
       <c r="H173" s="60" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.25">
@@ -10941,7 +10941,7 @@
         <v>142</v>
       </c>
       <c r="C174" s="52" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="D174" s="51" t="s">
         <v>267</v>
@@ -10954,7 +10954,7 @@
         <v>5</v>
       </c>
       <c r="H174" s="60" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="175" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10965,10 +10965,10 @@
         <v>140</v>
       </c>
       <c r="C175" s="101" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="D175" s="125" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E175" s="100" t="s">
         <v>264</v>
@@ -10980,7 +10980,7 @@
         <v>5</v>
       </c>
       <c r="H175" s="126" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.25">
@@ -10991,7 +10991,7 @@
         <v>140</v>
       </c>
       <c r="C176" s="106" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D176" s="107" t="s">
         <v>258</v>
@@ -11004,7 +11004,7 @@
       </c>
       <c r="G176" s="105"/>
       <c r="H176" s="108" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.25">
@@ -11015,7 +11015,7 @@
         <v>141</v>
       </c>
       <c r="C177" s="111" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D177" s="112" t="s">
         <v>260</v>
@@ -11030,7 +11030,7 @@
         <v>5</v>
       </c>
       <c r="H177" s="113" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.25">
@@ -11041,7 +11041,7 @@
         <v>142</v>
       </c>
       <c r="C178" s="111" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="D178" s="112" t="s">
         <v>259</v>
@@ -11059,7 +11059,7 @@
         <v>140</v>
       </c>
       <c r="C179" s="111" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D179" s="112" t="s">
         <v>261</v>
@@ -11074,7 +11074,7 @@
         <v>5</v>
       </c>
       <c r="H179" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.25">
@@ -11085,7 +11085,7 @@
         <v>143</v>
       </c>
       <c r="C180" s="111" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D180" s="112" t="s">
         <v>262</v>
@@ -11100,7 +11100,7 @@
         <v>5</v>
       </c>
       <c r="H180" s="113" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.25">
@@ -11111,7 +11111,7 @@
         <v>142</v>
       </c>
       <c r="C181" s="111" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="D181" s="112" t="s">
         <v>263</v>
@@ -11124,7 +11124,7 @@
         <v>5</v>
       </c>
       <c r="H181" s="113" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
     <row r="182" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11135,10 +11135,10 @@
         <v>140</v>
       </c>
       <c r="C182" s="116" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="D182" s="117" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E182" s="115" t="s">
         <v>125</v>
@@ -11150,7 +11150,7 @@
         <v>5</v>
       </c>
       <c r="H182" s="118" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
     </row>
   </sheetData>
@@ -11187,48 +11187,48 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="165" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B1" s="166"/>
       <c r="C1" s="167"/>
       <c r="E1" s="165" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F1" s="166"/>
       <c r="G1" s="167"/>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
+        <v>315</v>
+      </c>
+      <c r="B2" s="78" t="s">
         <v>316</v>
       </c>
-      <c r="B2" s="78" t="s">
+      <c r="C2" s="79" t="s">
         <v>317</v>
       </c>
-      <c r="C2" s="79" t="s">
-        <v>318</v>
-      </c>
       <c r="E2" s="77" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F2" s="78" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="G2" s="79" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="B3" s="68" t="s">
+        <v>320</v>
+      </c>
+      <c r="C3" s="69" t="s">
         <v>321</v>
       </c>
-      <c r="C3" s="69" t="s">
-        <v>322</v>
-      </c>
       <c r="E3" s="67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="F3" s="68"/>
       <c r="G3" s="69"/>
@@ -11236,10 +11236,10 @@
     <row r="4" spans="1:7" ht="90" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="70"/>
       <c r="B4" s="71" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="C4" s="72" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="E4" s="70"/>
       <c r="F4" s="71"/>
@@ -11255,13 +11255,13 @@
     </row>
     <row r="6" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="67" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B6" s="68" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" s="69" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E6" s="67"/>
       <c r="F6" s="68"/>
@@ -11270,10 +11270,10 @@
     <row r="7" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A7" s="73"/>
       <c r="B7" s="9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C7" s="74" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E7" s="73"/>
       <c r="F7" s="9"/>
@@ -11282,10 +11282,10 @@
     <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="73"/>
       <c r="B8" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C8" s="74" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E8" s="73"/>
       <c r="F8" s="9"/>
@@ -11294,10 +11294,10 @@
     <row r="9" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="73"/>
       <c r="B9" s="9" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C9" s="74" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E9" s="73"/>
       <c r="F9" s="9"/>
@@ -11306,10 +11306,10 @@
     <row r="10" spans="1:7" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="70"/>
       <c r="B10" s="71" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C10" s="72" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E10" s="70"/>
       <c r="F10" s="71"/>
@@ -11325,7 +11325,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="75" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B12" s="75"/>
       <c r="C12" s="75"/>

</xml_diff>